<commit_message>
--IA & WBS Completed--
</commit_message>
<xml_diff>
--- a/amazon_wbs.xlsx
+++ b/amazon_wbs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyler\OneDrive\문서\Ezenac\Project 02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ezenac\Project02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB10C0BF-525F-467C-9CFE-62EC860ECDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81C76BE-ACD0-4FC8-8207-9D61C7E70BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="8055" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="62">
   <si>
     <t>프로젝트 이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -245,6 +245,26 @@
   </si>
   <si>
     <t>프레젠테이션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김효인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김예지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해오름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>박제한</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마이페이지</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -381,7 +401,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="73">
+  <borders count="78">
     <border>
       <left/>
       <right/>
@@ -1315,6 +1335,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1333,7 +1412,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1547,48 +1626,60 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="26" xfId="4" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="30" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="31" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="36" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1604,43 +1695,43 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="30" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="31" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="37" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="38" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="39" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1658,23 +1749,38 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="37" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="38" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="39" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1960,13 +2066,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DY50"/>
+  <dimension ref="A1:DY54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="2.625" customWidth="1"/>
     <col min="2" max="2" width="20.625" style="1" customWidth="1"/>
@@ -1977,8 +2083,8 @@
     <col min="52" max="63" width="6.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:129" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:129" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:129" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.65"/>
+    <row r="2" spans="1:129" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1986,7 +2092,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:129" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:129" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
@@ -1994,7 +2100,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:129" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:129" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B4" s="9" t="s">
         <v>3</v>
       </c>
@@ -2002,75 +2108,75 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:129" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:129" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="111" t="s">
+      <c r="J5" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="112"/>
-      <c r="L5" s="112"/>
-      <c r="M5" s="112"/>
-      <c r="N5" s="112"/>
-      <c r="O5" s="112"/>
-      <c r="P5" s="112"/>
-      <c r="Q5" s="112"/>
-      <c r="R5" s="112"/>
-      <c r="S5" s="112"/>
-      <c r="T5" s="112"/>
-      <c r="U5" s="112"/>
-      <c r="V5" s="112"/>
-      <c r="W5" s="112"/>
-      <c r="X5" s="112"/>
-      <c r="Y5" s="112"/>
-      <c r="Z5" s="113"/>
-      <c r="AA5" s="85" t="s">
+      <c r="K5" s="103"/>
+      <c r="L5" s="103"/>
+      <c r="M5" s="103"/>
+      <c r="N5" s="103"/>
+      <c r="O5" s="103"/>
+      <c r="P5" s="103"/>
+      <c r="Q5" s="103"/>
+      <c r="R5" s="103"/>
+      <c r="S5" s="103"/>
+      <c r="T5" s="103"/>
+      <c r="U5" s="103"/>
+      <c r="V5" s="103"/>
+      <c r="W5" s="103"/>
+      <c r="X5" s="103"/>
+      <c r="Y5" s="103"/>
+      <c r="Z5" s="104"/>
+      <c r="AA5" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="AB5" s="86"/>
-      <c r="AC5" s="86"/>
-      <c r="AD5" s="86"/>
-      <c r="AE5" s="86"/>
-      <c r="AF5" s="86"/>
-      <c r="AG5" s="86"/>
-      <c r="AH5" s="86"/>
-      <c r="AI5" s="86"/>
-      <c r="AJ5" s="86"/>
-      <c r="AK5" s="86"/>
-      <c r="AL5" s="86"/>
-      <c r="AM5" s="86"/>
-      <c r="AN5" s="86"/>
-      <c r="AO5" s="86"/>
-      <c r="AP5" s="86"/>
-      <c r="AQ5" s="86"/>
-      <c r="AR5" s="86"/>
-      <c r="AS5" s="86"/>
-      <c r="AT5" s="86"/>
-      <c r="AU5" s="86"/>
-      <c r="AV5" s="86"/>
-      <c r="AW5" s="86"/>
-      <c r="AX5" s="86"/>
-      <c r="AY5" s="86"/>
-      <c r="AZ5" s="86"/>
-      <c r="BA5" s="86"/>
-      <c r="BB5" s="86"/>
-      <c r="BC5" s="86"/>
-      <c r="BD5" s="86"/>
-      <c r="BE5" s="87"/>
-      <c r="BF5" s="88" t="s">
+      <c r="AB5" s="90"/>
+      <c r="AC5" s="90"/>
+      <c r="AD5" s="90"/>
+      <c r="AE5" s="90"/>
+      <c r="AF5" s="90"/>
+      <c r="AG5" s="90"/>
+      <c r="AH5" s="90"/>
+      <c r="AI5" s="90"/>
+      <c r="AJ5" s="90"/>
+      <c r="AK5" s="90"/>
+      <c r="AL5" s="90"/>
+      <c r="AM5" s="90"/>
+      <c r="AN5" s="90"/>
+      <c r="AO5" s="90"/>
+      <c r="AP5" s="90"/>
+      <c r="AQ5" s="90"/>
+      <c r="AR5" s="90"/>
+      <c r="AS5" s="90"/>
+      <c r="AT5" s="90"/>
+      <c r="AU5" s="90"/>
+      <c r="AV5" s="90"/>
+      <c r="AW5" s="90"/>
+      <c r="AX5" s="90"/>
+      <c r="AY5" s="90"/>
+      <c r="AZ5" s="90"/>
+      <c r="BA5" s="90"/>
+      <c r="BB5" s="90"/>
+      <c r="BC5" s="90"/>
+      <c r="BD5" s="90"/>
+      <c r="BE5" s="91"/>
+      <c r="BF5" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="BG5" s="89"/>
-      <c r="BH5" s="89"/>
-      <c r="BI5" s="89"/>
-      <c r="BJ5" s="89"/>
-      <c r="BK5" s="89"/>
+      <c r="BG5" s="93"/>
+      <c r="BH5" s="93"/>
+      <c r="BI5" s="93"/>
+      <c r="BJ5" s="93"/>
+      <c r="BK5" s="93"/>
     </row>
-    <row r="6" spans="1:129" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:129" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="J6" s="1">
         <v>15</v>
       </c>
@@ -2234,109 +2340,109 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:129" s="31" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:129" s="31" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A7"/>
-      <c r="B7" s="90" t="s">
+      <c r="B7" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="90" t="s">
+      <c r="C7" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="90" t="s">
+      <c r="D7" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90" t="s">
+      <c r="E7" s="72"/>
+      <c r="F7" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="90" t="s">
+      <c r="G7" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="90" t="s">
+      <c r="H7" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="109" t="s">
+      <c r="I7" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="93" t="s">
+      <c r="J7" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="94"/>
-      <c r="L7" s="94"/>
-      <c r="M7" s="94"/>
-      <c r="N7" s="94"/>
-      <c r="O7" s="94"/>
-      <c r="P7" s="94"/>
-      <c r="Q7" s="93" t="s">
+      <c r="K7" s="76"/>
+      <c r="L7" s="76"/>
+      <c r="M7" s="76"/>
+      <c r="N7" s="76"/>
+      <c r="O7" s="76"/>
+      <c r="P7" s="76"/>
+      <c r="Q7" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="R7" s="94"/>
-      <c r="S7" s="94"/>
-      <c r="T7" s="94"/>
-      <c r="U7" s="94"/>
-      <c r="V7" s="94"/>
-      <c r="W7" s="94"/>
-      <c r="X7" s="93" t="s">
+      <c r="R7" s="76"/>
+      <c r="S7" s="76"/>
+      <c r="T7" s="76"/>
+      <c r="U7" s="76"/>
+      <c r="V7" s="76"/>
+      <c r="W7" s="76"/>
+      <c r="X7" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="Y7" s="94"/>
-      <c r="Z7" s="94"/>
-      <c r="AA7" s="94"/>
-      <c r="AB7" s="94"/>
-      <c r="AC7" s="94"/>
-      <c r="AD7" s="94"/>
-      <c r="AE7" s="93" t="s">
+      <c r="Y7" s="76"/>
+      <c r="Z7" s="76"/>
+      <c r="AA7" s="76"/>
+      <c r="AB7" s="76"/>
+      <c r="AC7" s="76"/>
+      <c r="AD7" s="76"/>
+      <c r="AE7" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="AF7" s="94"/>
-      <c r="AG7" s="94"/>
-      <c r="AH7" s="94"/>
-      <c r="AI7" s="94"/>
-      <c r="AJ7" s="94"/>
-      <c r="AK7" s="94"/>
-      <c r="AL7" s="93" t="s">
+      <c r="AF7" s="76"/>
+      <c r="AG7" s="76"/>
+      <c r="AH7" s="76"/>
+      <c r="AI7" s="76"/>
+      <c r="AJ7" s="76"/>
+      <c r="AK7" s="76"/>
+      <c r="AL7" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="AM7" s="94"/>
-      <c r="AN7" s="94"/>
-      <c r="AO7" s="94"/>
-      <c r="AP7" s="94"/>
-      <c r="AQ7" s="94"/>
-      <c r="AR7" s="94"/>
-      <c r="AS7" s="93" t="s">
+      <c r="AM7" s="76"/>
+      <c r="AN7" s="76"/>
+      <c r="AO7" s="76"/>
+      <c r="AP7" s="76"/>
+      <c r="AQ7" s="76"/>
+      <c r="AR7" s="76"/>
+      <c r="AS7" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="AT7" s="94"/>
-      <c r="AU7" s="94"/>
-      <c r="AV7" s="94"/>
-      <c r="AW7" s="94"/>
-      <c r="AX7" s="94"/>
-      <c r="AY7" s="94"/>
-      <c r="AZ7" s="93" t="s">
+      <c r="AT7" s="76"/>
+      <c r="AU7" s="76"/>
+      <c r="AV7" s="76"/>
+      <c r="AW7" s="76"/>
+      <c r="AX7" s="76"/>
+      <c r="AY7" s="76"/>
+      <c r="AZ7" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="BA7" s="94"/>
-      <c r="BB7" s="94"/>
-      <c r="BC7" s="94"/>
-      <c r="BD7" s="94"/>
-      <c r="BE7" s="94"/>
-      <c r="BF7" s="94"/>
-      <c r="BG7" s="93" t="s">
+      <c r="BA7" s="76"/>
+      <c r="BB7" s="76"/>
+      <c r="BC7" s="76"/>
+      <c r="BD7" s="76"/>
+      <c r="BE7" s="76"/>
+      <c r="BF7" s="76"/>
+      <c r="BG7" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="BH7" s="94"/>
-      <c r="BI7" s="94"/>
-      <c r="BJ7" s="94"/>
-      <c r="BK7" s="94"/>
+      <c r="BH7" s="76"/>
+      <c r="BI7" s="76"/>
+      <c r="BJ7" s="76"/>
+      <c r="BK7" s="76"/>
       <c r="BL7"/>
       <c r="BM7"/>
-      <c r="BN7" s="84"/>
-      <c r="BO7" s="84"/>
-      <c r="BP7" s="84"/>
-      <c r="BQ7" s="84"/>
-      <c r="BR7" s="84"/>
-      <c r="BS7" s="84"/>
-      <c r="BT7" s="84"/>
+      <c r="BN7" s="74"/>
+      <c r="BO7" s="74"/>
+      <c r="BP7" s="74"/>
+      <c r="BQ7" s="74"/>
+      <c r="BR7" s="74"/>
+      <c r="BS7" s="74"/>
+      <c r="BT7" s="74"/>
       <c r="BU7"/>
       <c r="BV7"/>
       <c r="BW7"/>
@@ -2395,16 +2501,16 @@
       <c r="DX7"/>
       <c r="DY7"/>
     </row>
-    <row r="8" spans="1:129" s="32" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:129" s="32" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A8"/>
-      <c r="B8" s="91"/>
-      <c r="C8" s="91"/>
-      <c r="D8" s="91"/>
-      <c r="E8" s="91"/>
-      <c r="F8" s="91"/>
-      <c r="G8" s="91"/>
-      <c r="H8" s="91"/>
-      <c r="I8" s="110"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="101"/>
       <c r="J8" s="31" t="s">
         <v>9</v>
       </c>
@@ -2634,18 +2740,18 @@
       <c r="DX8"/>
       <c r="DY8"/>
     </row>
-    <row r="9" spans="1:129" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:129" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.6">
       <c r="B9" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="95" t="s">
+      <c r="D9" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="96"/>
-      <c r="F9" s="82" t="s">
+      <c r="E9" s="78"/>
+      <c r="F9" s="94" t="s">
         <v>42</v>
       </c>
       <c r="G9" s="3">
@@ -2712,14 +2818,14 @@
       <c r="BJ9" s="19"/>
       <c r="BK9" s="60"/>
     </row>
-    <row r="10" spans="1:129" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:129" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B10" s="13"/>
       <c r="C10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="97"/>
-      <c r="E10" s="98"/>
-      <c r="F10" s="72"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="95"/>
       <c r="G10" s="3">
         <v>45486</v>
       </c>
@@ -2784,14 +2890,14 @@
       <c r="BJ10" s="21"/>
       <c r="BK10" s="61"/>
     </row>
-    <row r="11" spans="1:129" s="33" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:129" s="33" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="B11" s="34"/>
       <c r="C11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="99"/>
-      <c r="E11" s="100"/>
-      <c r="F11" s="83"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="96"/>
       <c r="G11" s="35">
         <v>45486</v>
       </c>
@@ -2922,15 +3028,15 @@
       <c r="DX11"/>
       <c r="DY11"/>
     </row>
-    <row r="12" spans="1:129" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:129" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B12" s="26" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="108"/>
-      <c r="E12" s="108"/>
+      <c r="D12" s="105"/>
+      <c r="E12" s="105"/>
       <c r="F12" s="16" t="s">
         <v>42</v>
       </c>
@@ -2998,22 +3104,22 @@
       <c r="BJ12" s="19"/>
       <c r="BK12" s="63"/>
     </row>
-    <row r="13" spans="1:129" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:129" ht="25.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B13" s="14"/>
-      <c r="C13" s="71" t="s">
+      <c r="C13" s="112" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="92" t="s">
+      <c r="D13" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="92"/>
+      <c r="E13" s="83"/>
       <c r="F13" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="74">
+      <c r="G13" s="97">
         <v>45491</v>
       </c>
-      <c r="H13" s="74">
+      <c r="H13" s="97">
         <v>45495</v>
       </c>
       <c r="I13" s="17">
@@ -3074,16 +3180,18 @@
       <c r="BJ13" s="21"/>
       <c r="BK13" s="61"/>
     </row>
-    <row r="14" spans="1:129" s="38" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:129" s="38" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B14" s="39"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="92" t="s">
+      <c r="C14" s="95"/>
+      <c r="D14" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="92"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="75"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="98"/>
+      <c r="H14" s="98"/>
       <c r="I14" s="41">
         <v>0</v>
       </c>
@@ -3208,16 +3316,18 @@
       <c r="DX14"/>
       <c r="DY14"/>
     </row>
-    <row r="15" spans="1:129" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:129" ht="25.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B15" s="39"/>
-      <c r="C15" s="72"/>
-      <c r="D15" s="92" t="s">
+      <c r="C15" s="95"/>
+      <c r="D15" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="92"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="75"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="98"/>
+      <c r="H15" s="98"/>
       <c r="I15" s="17">
         <v>0</v>
       </c>
@@ -3276,16 +3386,18 @@
       <c r="BJ15" s="19"/>
       <c r="BK15" s="63"/>
     </row>
-    <row r="16" spans="1:129" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:129" ht="25.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B16" s="39"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="92" t="s">
+      <c r="C16" s="95"/>
+      <c r="D16" s="83" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="92"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="75"/>
-      <c r="H16" s="75"/>
+      <c r="E16" s="83"/>
+      <c r="F16" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="98"/>
+      <c r="H16" s="98"/>
       <c r="I16" s="17">
         <v>0</v>
       </c>
@@ -3344,16 +3456,18 @@
       <c r="BJ16" s="21"/>
       <c r="BK16" s="61"/>
     </row>
-    <row r="17" spans="2:129" s="38" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:129" s="38" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B17" s="39"/>
-      <c r="C17" s="72"/>
-      <c r="D17" s="101" t="s">
+      <c r="C17" s="95"/>
+      <c r="D17" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="101"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
+      <c r="E17" s="84"/>
+      <c r="F17" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="98"/>
+      <c r="H17" s="98"/>
       <c r="I17" s="45">
         <v>0</v>
       </c>
@@ -3478,73 +3592,75 @@
       <c r="DX17"/>
       <c r="DY17"/>
     </row>
-    <row r="18" spans="2:129" s="29" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="30"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="73"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="76"/>
-      <c r="H18" s="76"/>
-      <c r="I18" s="47">
+    <row r="18" spans="2:129" s="115" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B18" s="119"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="84" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="84"/>
+      <c r="F18" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="98"/>
+      <c r="H18" s="98"/>
+      <c r="I18" s="45">
         <v>0</v>
       </c>
-      <c r="J18" s="48"/>
-      <c r="K18" s="49"/>
-      <c r="L18" s="49"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="49"/>
-      <c r="O18" s="49"/>
-      <c r="P18" s="49"/>
-      <c r="Q18" s="48"/>
-      <c r="R18" s="49"/>
-      <c r="S18" s="49"/>
-      <c r="T18" s="49"/>
-      <c r="U18" s="49"/>
-      <c r="V18" s="49"/>
-      <c r="W18" s="49"/>
-      <c r="X18" s="48"/>
-      <c r="Y18" s="49"/>
-      <c r="Z18" s="49"/>
-      <c r="AA18" s="49"/>
-      <c r="AB18" s="49"/>
-      <c r="AC18" s="49"/>
-      <c r="AD18" s="49"/>
-      <c r="AE18" s="48"/>
-      <c r="AF18" s="49"/>
-      <c r="AG18" s="49"/>
-      <c r="AH18" s="49"/>
-      <c r="AI18" s="49"/>
-      <c r="AJ18" s="49"/>
-      <c r="AK18" s="49"/>
-      <c r="AL18" s="48"/>
-      <c r="AM18" s="49"/>
-      <c r="AN18" s="49"/>
-      <c r="AO18" s="49"/>
-      <c r="AP18" s="49"/>
-      <c r="AQ18" s="49"/>
-      <c r="AR18" s="49"/>
-      <c r="AS18" s="48"/>
-      <c r="AT18" s="49"/>
-      <c r="AU18" s="49"/>
-      <c r="AV18" s="49"/>
-      <c r="AW18" s="49"/>
-      <c r="AX18" s="49"/>
-      <c r="AY18" s="49"/>
-      <c r="AZ18" s="48"/>
-      <c r="BA18" s="49"/>
-      <c r="BB18" s="49"/>
-      <c r="BC18" s="49"/>
-      <c r="BD18" s="49"/>
-      <c r="BE18" s="49"/>
-      <c r="BF18" s="49"/>
-      <c r="BG18" s="48"/>
-      <c r="BH18" s="49"/>
-      <c r="BI18" s="49"/>
-      <c r="BJ18" s="49"/>
-      <c r="BK18" s="65"/>
+      <c r="J18" s="116"/>
+      <c r="K18" s="117"/>
+      <c r="L18" s="117"/>
+      <c r="M18" s="117"/>
+      <c r="N18" s="117"/>
+      <c r="O18" s="117"/>
+      <c r="P18" s="117"/>
+      <c r="Q18" s="116"/>
+      <c r="R18" s="117"/>
+      <c r="S18" s="117"/>
+      <c r="T18" s="117"/>
+      <c r="U18" s="117"/>
+      <c r="V18" s="117"/>
+      <c r="W18" s="117"/>
+      <c r="X18" s="116"/>
+      <c r="Y18" s="117"/>
+      <c r="Z18" s="117"/>
+      <c r="AA18" s="117"/>
+      <c r="AB18" s="117"/>
+      <c r="AC18" s="117"/>
+      <c r="AD18" s="117"/>
+      <c r="AE18" s="116"/>
+      <c r="AF18" s="117"/>
+      <c r="AG18" s="117"/>
+      <c r="AH18" s="117"/>
+      <c r="AI18" s="117"/>
+      <c r="AJ18" s="117"/>
+      <c r="AK18" s="117"/>
+      <c r="AL18" s="116"/>
+      <c r="AM18" s="117"/>
+      <c r="AN18" s="117"/>
+      <c r="AO18" s="117"/>
+      <c r="AP18" s="117"/>
+      <c r="AQ18" s="117"/>
+      <c r="AR18" s="117"/>
+      <c r="AS18" s="116"/>
+      <c r="AT18" s="117"/>
+      <c r="AU18" s="117"/>
+      <c r="AV18" s="117"/>
+      <c r="AW18" s="117"/>
+      <c r="AX18" s="117"/>
+      <c r="AY18" s="117"/>
+      <c r="AZ18" s="116"/>
+      <c r="BA18" s="117"/>
+      <c r="BB18" s="117"/>
+      <c r="BC18" s="117"/>
+      <c r="BD18" s="117"/>
+      <c r="BE18" s="117"/>
+      <c r="BF18" s="117"/>
+      <c r="BG18" s="116"/>
+      <c r="BH18" s="117"/>
+      <c r="BI18" s="117"/>
+      <c r="BJ18" s="117"/>
+      <c r="BK18" s="118"/>
       <c r="BL18"/>
       <c r="BM18"/>
       <c r="BN18"/>
@@ -3612,158 +3728,230 @@
       <c r="DX18"/>
       <c r="DY18"/>
     </row>
-    <row r="19" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="44"/>
-      <c r="C19" s="82" t="s">
+    <row r="19" spans="2:129" s="29" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B19" s="30"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="85" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="85"/>
+      <c r="F19" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="99"/>
+      <c r="H19" s="99"/>
+      <c r="I19" s="47">
+        <v>0</v>
+      </c>
+      <c r="J19" s="48"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="49"/>
+      <c r="N19" s="49"/>
+      <c r="O19" s="49"/>
+      <c r="P19" s="49"/>
+      <c r="Q19" s="48"/>
+      <c r="R19" s="49"/>
+      <c r="S19" s="49"/>
+      <c r="T19" s="49"/>
+      <c r="U19" s="49"/>
+      <c r="V19" s="49"/>
+      <c r="W19" s="49"/>
+      <c r="X19" s="48"/>
+      <c r="Y19" s="49"/>
+      <c r="Z19" s="49"/>
+      <c r="AA19" s="49"/>
+      <c r="AB19" s="49"/>
+      <c r="AC19" s="49"/>
+      <c r="AD19" s="49"/>
+      <c r="AE19" s="48"/>
+      <c r="AF19" s="49"/>
+      <c r="AG19" s="49"/>
+      <c r="AH19" s="49"/>
+      <c r="AI19" s="49"/>
+      <c r="AJ19" s="49"/>
+      <c r="AK19" s="49"/>
+      <c r="AL19" s="48"/>
+      <c r="AM19" s="49"/>
+      <c r="AN19" s="49"/>
+      <c r="AO19" s="49"/>
+      <c r="AP19" s="49"/>
+      <c r="AQ19" s="49"/>
+      <c r="AR19" s="49"/>
+      <c r="AS19" s="48"/>
+      <c r="AT19" s="49"/>
+      <c r="AU19" s="49"/>
+      <c r="AV19" s="49"/>
+      <c r="AW19" s="49"/>
+      <c r="AX19" s="49"/>
+      <c r="AY19" s="49"/>
+      <c r="AZ19" s="48"/>
+      <c r="BA19" s="49"/>
+      <c r="BB19" s="49"/>
+      <c r="BC19" s="49"/>
+      <c r="BD19" s="49"/>
+      <c r="BE19" s="49"/>
+      <c r="BF19" s="49"/>
+      <c r="BG19" s="48"/>
+      <c r="BH19" s="49"/>
+      <c r="BI19" s="49"/>
+      <c r="BJ19" s="49"/>
+      <c r="BK19" s="65"/>
+      <c r="BL19"/>
+      <c r="BM19"/>
+      <c r="BN19"/>
+      <c r="BO19"/>
+      <c r="BP19"/>
+      <c r="BQ19"/>
+      <c r="BR19"/>
+      <c r="BS19"/>
+      <c r="BT19"/>
+      <c r="BU19"/>
+      <c r="BV19"/>
+      <c r="BW19"/>
+      <c r="BX19"/>
+      <c r="BY19"/>
+      <c r="BZ19"/>
+      <c r="CA19"/>
+      <c r="CB19"/>
+      <c r="CC19"/>
+      <c r="CD19"/>
+      <c r="CE19"/>
+      <c r="CF19"/>
+      <c r="CG19"/>
+      <c r="CH19"/>
+      <c r="CI19"/>
+      <c r="CJ19"/>
+      <c r="CK19"/>
+      <c r="CL19"/>
+      <c r="CM19"/>
+      <c r="CN19"/>
+      <c r="CO19"/>
+      <c r="CP19"/>
+      <c r="CQ19"/>
+      <c r="CR19"/>
+      <c r="CS19"/>
+      <c r="CT19"/>
+      <c r="CU19"/>
+      <c r="CV19"/>
+      <c r="CW19"/>
+      <c r="CX19"/>
+      <c r="CY19"/>
+      <c r="CZ19"/>
+      <c r="DA19"/>
+      <c r="DB19"/>
+      <c r="DC19"/>
+      <c r="DD19"/>
+      <c r="DE19"/>
+      <c r="DF19"/>
+      <c r="DG19"/>
+      <c r="DH19"/>
+      <c r="DI19"/>
+      <c r="DJ19"/>
+      <c r="DK19"/>
+      <c r="DL19"/>
+      <c r="DM19"/>
+      <c r="DN19"/>
+      <c r="DO19"/>
+      <c r="DP19"/>
+      <c r="DQ19"/>
+      <c r="DR19"/>
+      <c r="DS19"/>
+      <c r="DT19"/>
+      <c r="DU19"/>
+      <c r="DV19"/>
+      <c r="DW19"/>
+      <c r="DX19"/>
+      <c r="DY19"/>
+    </row>
+    <row r="20" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B20" s="44"/>
+      <c r="C20" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="108" t="s">
+      <c r="D20" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="108"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="77">
+      <c r="E20" s="105"/>
+      <c r="F20" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="106">
         <v>45495</v>
       </c>
-      <c r="H19" s="77">
+      <c r="H20" s="106">
         <v>45499</v>
       </c>
-      <c r="I19" s="17">
-        <v>0</v>
-      </c>
-      <c r="J19" s="18"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="19"/>
-      <c r="S19" s="19"/>
-      <c r="T19" s="19"/>
-      <c r="U19" s="19"/>
-      <c r="V19" s="19"/>
-      <c r="W19" s="20"/>
-      <c r="X19" s="18"/>
-      <c r="Y19" s="19"/>
-      <c r="Z19" s="19"/>
-      <c r="AA19" s="19"/>
-      <c r="AB19" s="19"/>
-      <c r="AC19" s="19"/>
-      <c r="AD19" s="20"/>
-      <c r="AE19" s="18"/>
-      <c r="AF19" s="19"/>
-      <c r="AG19" s="19"/>
-      <c r="AH19" s="19"/>
-      <c r="AI19" s="19"/>
-      <c r="AJ19" s="19"/>
-      <c r="AK19" s="20"/>
-      <c r="AL19" s="18"/>
-      <c r="AM19" s="19"/>
-      <c r="AN19" s="19"/>
-      <c r="AO19" s="19"/>
-      <c r="AP19" s="19"/>
-      <c r="AQ19" s="19"/>
-      <c r="AR19" s="20"/>
-      <c r="AS19" s="18"/>
-      <c r="AT19" s="19"/>
-      <c r="AU19" s="19"/>
-      <c r="AV19" s="19"/>
-      <c r="AW19" s="19"/>
-      <c r="AX19" s="19"/>
-      <c r="AY19" s="20"/>
-      <c r="AZ19" s="18"/>
-      <c r="BA19" s="19"/>
-      <c r="BB19" s="19"/>
-      <c r="BC19" s="19"/>
-      <c r="BD19" s="19"/>
-      <c r="BE19" s="19"/>
-      <c r="BF19" s="20"/>
-      <c r="BG19" s="18"/>
-      <c r="BH19" s="19"/>
-      <c r="BI19" s="19"/>
-      <c r="BJ19" s="19"/>
-      <c r="BK19" s="63"/>
-    </row>
-    <row r="20" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="14"/>
-      <c r="C20" s="72"/>
-      <c r="D20" s="92" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="92"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="75"/>
-      <c r="H20" s="75"/>
       <c r="I20" s="17">
         <v>0</v>
       </c>
-      <c r="J20" s="23"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="21"/>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="21"/>
-      <c r="S20" s="21"/>
-      <c r="T20" s="21"/>
-      <c r="U20" s="21"/>
-      <c r="V20" s="21"/>
-      <c r="W20" s="21"/>
-      <c r="X20" s="23"/>
-      <c r="Y20" s="21"/>
-      <c r="Z20" s="21"/>
-      <c r="AA20" s="21"/>
-      <c r="AB20" s="21"/>
-      <c r="AC20" s="21"/>
-      <c r="AD20" s="21"/>
-      <c r="AE20" s="23"/>
-      <c r="AF20" s="21"/>
-      <c r="AG20" s="21"/>
-      <c r="AH20" s="21"/>
-      <c r="AI20" s="21"/>
-      <c r="AJ20" s="21"/>
-      <c r="AK20" s="21"/>
-      <c r="AL20" s="23"/>
-      <c r="AM20" s="21"/>
-      <c r="AN20" s="21"/>
-      <c r="AO20" s="21"/>
-      <c r="AP20" s="21"/>
-      <c r="AQ20" s="21"/>
-      <c r="AR20" s="21"/>
-      <c r="AS20" s="23"/>
-      <c r="AT20" s="21"/>
-      <c r="AU20" s="21"/>
-      <c r="AV20" s="21"/>
-      <c r="AW20" s="21"/>
-      <c r="AX20" s="21"/>
-      <c r="AY20" s="21"/>
-      <c r="AZ20" s="23"/>
-      <c r="BA20" s="21"/>
-      <c r="BB20" s="21"/>
-      <c r="BC20" s="21"/>
-      <c r="BD20" s="21"/>
-      <c r="BE20" s="21"/>
-      <c r="BF20" s="21"/>
-      <c r="BG20" s="23"/>
-      <c r="BH20" s="21"/>
-      <c r="BI20" s="21"/>
-      <c r="BJ20" s="21"/>
-      <c r="BK20" s="61"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="19"/>
+      <c r="U20" s="19"/>
+      <c r="V20" s="19"/>
+      <c r="W20" s="20"/>
+      <c r="X20" s="18"/>
+      <c r="Y20" s="19"/>
+      <c r="Z20" s="19"/>
+      <c r="AA20" s="19"/>
+      <c r="AB20" s="19"/>
+      <c r="AC20" s="19"/>
+      <c r="AD20" s="20"/>
+      <c r="AE20" s="18"/>
+      <c r="AF20" s="19"/>
+      <c r="AG20" s="19"/>
+      <c r="AH20" s="19"/>
+      <c r="AI20" s="19"/>
+      <c r="AJ20" s="19"/>
+      <c r="AK20" s="20"/>
+      <c r="AL20" s="18"/>
+      <c r="AM20" s="19"/>
+      <c r="AN20" s="19"/>
+      <c r="AO20" s="19"/>
+      <c r="AP20" s="19"/>
+      <c r="AQ20" s="19"/>
+      <c r="AR20" s="20"/>
+      <c r="AS20" s="18"/>
+      <c r="AT20" s="19"/>
+      <c r="AU20" s="19"/>
+      <c r="AV20" s="19"/>
+      <c r="AW20" s="19"/>
+      <c r="AX20" s="19"/>
+      <c r="AY20" s="20"/>
+      <c r="AZ20" s="18"/>
+      <c r="BA20" s="19"/>
+      <c r="BB20" s="19"/>
+      <c r="BC20" s="19"/>
+      <c r="BD20" s="19"/>
+      <c r="BE20" s="19"/>
+      <c r="BF20" s="20"/>
+      <c r="BG20" s="18"/>
+      <c r="BH20" s="19"/>
+      <c r="BI20" s="19"/>
+      <c r="BJ20" s="19"/>
+      <c r="BK20" s="63"/>
     </row>
-    <row r="21" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B21" s="14"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="92" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="92"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="75"/>
-      <c r="H21" s="75"/>
+      <c r="C21" s="95"/>
+      <c r="D21" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="83"/>
+      <c r="F21" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" s="98"/>
+      <c r="H21" s="98"/>
       <c r="I21" s="17">
         <v>0</v>
       </c>
@@ -3822,16 +4010,18 @@
       <c r="BJ21" s="21"/>
       <c r="BK21" s="61"/>
     </row>
-    <row r="22" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B22" s="14"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="92" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="92"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="75"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="83" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="83"/>
+      <c r="F22" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" s="98"/>
+      <c r="H22" s="98"/>
       <c r="I22" s="17">
         <v>0</v>
       </c>
@@ -3890,16 +4080,18 @@
       <c r="BJ22" s="21"/>
       <c r="BK22" s="61"/>
     </row>
-    <row r="23" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B23" s="14"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="101" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="101"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="75"/>
-      <c r="H23" s="75"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="83" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="83"/>
+      <c r="F23" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="98"/>
+      <c r="H23" s="98"/>
       <c r="I23" s="17">
         <v>0</v>
       </c>
@@ -3958,508 +4150,516 @@
       <c r="BJ23" s="21"/>
       <c r="BK23" s="61"/>
     </row>
-    <row r="24" spans="2:129" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="30"/>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73" t="s">
+    <row r="24" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B24" s="14"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="84"/>
+      <c r="F24" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G24" s="98"/>
+      <c r="H24" s="98"/>
+      <c r="I24" s="17">
+        <v>0</v>
+      </c>
+      <c r="J24" s="23"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="21"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="21"/>
+      <c r="S24" s="21"/>
+      <c r="T24" s="21"/>
+      <c r="U24" s="21"/>
+      <c r="V24" s="21"/>
+      <c r="W24" s="21"/>
+      <c r="X24" s="23"/>
+      <c r="Y24" s="21"/>
+      <c r="Z24" s="21"/>
+      <c r="AA24" s="21"/>
+      <c r="AB24" s="21"/>
+      <c r="AC24" s="21"/>
+      <c r="AD24" s="21"/>
+      <c r="AE24" s="23"/>
+      <c r="AF24" s="21"/>
+      <c r="AG24" s="21"/>
+      <c r="AH24" s="21"/>
+      <c r="AI24" s="21"/>
+      <c r="AJ24" s="21"/>
+      <c r="AK24" s="21"/>
+      <c r="AL24" s="23"/>
+      <c r="AM24" s="21"/>
+      <c r="AN24" s="21"/>
+      <c r="AO24" s="21"/>
+      <c r="AP24" s="21"/>
+      <c r="AQ24" s="21"/>
+      <c r="AR24" s="21"/>
+      <c r="AS24" s="23"/>
+      <c r="AT24" s="21"/>
+      <c r="AU24" s="21"/>
+      <c r="AV24" s="21"/>
+      <c r="AW24" s="21"/>
+      <c r="AX24" s="21"/>
+      <c r="AY24" s="21"/>
+      <c r="AZ24" s="23"/>
+      <c r="BA24" s="21"/>
+      <c r="BB24" s="21"/>
+      <c r="BC24" s="21"/>
+      <c r="BD24" s="21"/>
+      <c r="BE24" s="21"/>
+      <c r="BF24" s="21"/>
+      <c r="BG24" s="23"/>
+      <c r="BH24" s="21"/>
+      <c r="BI24" s="21"/>
+      <c r="BJ24" s="21"/>
+      <c r="BK24" s="61"/>
+    </row>
+    <row r="25" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B25" s="119"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="84"/>
+      <c r="F25" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="98"/>
+      <c r="H25" s="98"/>
+      <c r="I25" s="17">
+        <v>0</v>
+      </c>
+      <c r="J25" s="120"/>
+      <c r="K25" s="121"/>
+      <c r="L25" s="121"/>
+      <c r="M25" s="121"/>
+      <c r="N25" s="121"/>
+      <c r="O25" s="121"/>
+      <c r="P25" s="121"/>
+      <c r="Q25" s="120"/>
+      <c r="R25" s="121"/>
+      <c r="S25" s="121"/>
+      <c r="T25" s="121"/>
+      <c r="U25" s="121"/>
+      <c r="V25" s="121"/>
+      <c r="W25" s="121"/>
+      <c r="X25" s="120"/>
+      <c r="Y25" s="121"/>
+      <c r="Z25" s="121"/>
+      <c r="AA25" s="121"/>
+      <c r="AB25" s="121"/>
+      <c r="AC25" s="121"/>
+      <c r="AD25" s="121"/>
+      <c r="AE25" s="120"/>
+      <c r="AF25" s="121"/>
+      <c r="AG25" s="121"/>
+      <c r="AH25" s="121"/>
+      <c r="AI25" s="121"/>
+      <c r="AJ25" s="121"/>
+      <c r="AK25" s="121"/>
+      <c r="AL25" s="120"/>
+      <c r="AM25" s="121"/>
+      <c r="AN25" s="121"/>
+      <c r="AO25" s="121"/>
+      <c r="AP25" s="121"/>
+      <c r="AQ25" s="121"/>
+      <c r="AR25" s="121"/>
+      <c r="AS25" s="120"/>
+      <c r="AT25" s="121"/>
+      <c r="AU25" s="121"/>
+      <c r="AV25" s="121"/>
+      <c r="AW25" s="121"/>
+      <c r="AX25" s="121"/>
+      <c r="AY25" s="121"/>
+      <c r="AZ25" s="120"/>
+      <c r="BA25" s="121"/>
+      <c r="BB25" s="121"/>
+      <c r="BC25" s="121"/>
+      <c r="BD25" s="121"/>
+      <c r="BE25" s="121"/>
+      <c r="BF25" s="121"/>
+      <c r="BG25" s="120"/>
+      <c r="BH25" s="121"/>
+      <c r="BI25" s="121"/>
+      <c r="BJ25" s="121"/>
+      <c r="BK25" s="122"/>
+    </row>
+    <row r="26" spans="2:129" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B26" s="30"/>
+      <c r="C26" s="85"/>
+      <c r="D26" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="73"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="76"/>
-      <c r="H24" s="76"/>
-      <c r="I24" s="47">
+      <c r="E26" s="85"/>
+      <c r="F26" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="99"/>
+      <c r="H26" s="99"/>
+      <c r="I26" s="47">
         <v>0</v>
       </c>
-      <c r="J24" s="27"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
-      <c r="O24" s="28"/>
-      <c r="P24" s="28"/>
-      <c r="Q24" s="27"/>
-      <c r="R24" s="28"/>
-      <c r="S24" s="28"/>
-      <c r="T24" s="28"/>
-      <c r="U24" s="28"/>
-      <c r="V24" s="28"/>
-      <c r="W24" s="28"/>
-      <c r="X24" s="27"/>
-      <c r="Y24" s="28"/>
-      <c r="Z24" s="28"/>
-      <c r="AA24" s="28"/>
-      <c r="AB24" s="28"/>
-      <c r="AC24" s="28"/>
-      <c r="AD24" s="28"/>
-      <c r="AE24" s="27"/>
-      <c r="AF24" s="28"/>
-      <c r="AG24" s="28"/>
-      <c r="AH24" s="28"/>
-      <c r="AI24" s="28"/>
-      <c r="AJ24" s="28"/>
-      <c r="AK24" s="28"/>
-      <c r="AL24" s="27"/>
-      <c r="AM24" s="28"/>
-      <c r="AN24" s="28"/>
-      <c r="AO24" s="28"/>
-      <c r="AP24" s="28"/>
-      <c r="AQ24" s="28"/>
-      <c r="AR24" s="28"/>
-      <c r="AS24" s="27"/>
-      <c r="AT24" s="28"/>
-      <c r="AU24" s="28"/>
-      <c r="AV24" s="28"/>
-      <c r="AW24" s="28"/>
-      <c r="AX24" s="28"/>
-      <c r="AY24" s="28"/>
-      <c r="AZ24" s="27"/>
-      <c r="BA24" s="28"/>
-      <c r="BB24" s="28"/>
-      <c r="BC24" s="28"/>
-      <c r="BD24" s="28"/>
-      <c r="BE24" s="28"/>
-      <c r="BF24" s="28"/>
-      <c r="BG24" s="27"/>
-      <c r="BH24" s="28"/>
-      <c r="BI24" s="28"/>
-      <c r="BJ24" s="28"/>
-      <c r="BK24" s="66"/>
-      <c r="BL24"/>
-      <c r="BM24"/>
-      <c r="BN24"/>
-      <c r="BO24"/>
-      <c r="BP24"/>
-      <c r="BQ24"/>
-      <c r="BR24"/>
-      <c r="BS24"/>
-      <c r="BT24"/>
-      <c r="BU24"/>
-      <c r="BV24"/>
-      <c r="BW24"/>
-      <c r="BX24"/>
-      <c r="BY24"/>
-      <c r="BZ24"/>
-      <c r="CA24"/>
-      <c r="CB24"/>
-      <c r="CC24"/>
-      <c r="CD24"/>
-      <c r="CE24"/>
-      <c r="CF24"/>
-      <c r="CG24"/>
-      <c r="CH24"/>
-      <c r="CI24"/>
-      <c r="CJ24"/>
-      <c r="CK24"/>
-      <c r="CL24"/>
-      <c r="CM24"/>
-      <c r="CN24"/>
-      <c r="CO24"/>
-      <c r="CP24"/>
-      <c r="CQ24"/>
-      <c r="CR24"/>
-      <c r="CS24"/>
-      <c r="CT24"/>
-      <c r="CU24"/>
-      <c r="CV24"/>
-      <c r="CW24"/>
-      <c r="CX24"/>
-      <c r="CY24"/>
-      <c r="CZ24"/>
-      <c r="DA24"/>
-      <c r="DB24"/>
-      <c r="DC24"/>
-      <c r="DD24"/>
-      <c r="DE24"/>
-      <c r="DF24"/>
-      <c r="DG24"/>
-      <c r="DH24"/>
-      <c r="DI24"/>
-      <c r="DJ24"/>
-      <c r="DK24"/>
-      <c r="DL24"/>
-      <c r="DM24"/>
-      <c r="DN24"/>
-      <c r="DO24"/>
-      <c r="DP24"/>
-      <c r="DQ24"/>
-      <c r="DR24"/>
-      <c r="DS24"/>
-      <c r="DT24"/>
-      <c r="DU24"/>
-      <c r="DV24"/>
-      <c r="DW24"/>
-      <c r="DX24"/>
-      <c r="DY24"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="28"/>
+      <c r="P26" s="28"/>
+      <c r="Q26" s="27"/>
+      <c r="R26" s="28"/>
+      <c r="S26" s="28"/>
+      <c r="T26" s="28"/>
+      <c r="U26" s="28"/>
+      <c r="V26" s="28"/>
+      <c r="W26" s="28"/>
+      <c r="X26" s="27"/>
+      <c r="Y26" s="28"/>
+      <c r="Z26" s="28"/>
+      <c r="AA26" s="28"/>
+      <c r="AB26" s="28"/>
+      <c r="AC26" s="28"/>
+      <c r="AD26" s="28"/>
+      <c r="AE26" s="27"/>
+      <c r="AF26" s="28"/>
+      <c r="AG26" s="28"/>
+      <c r="AH26" s="28"/>
+      <c r="AI26" s="28"/>
+      <c r="AJ26" s="28"/>
+      <c r="AK26" s="28"/>
+      <c r="AL26" s="27"/>
+      <c r="AM26" s="28"/>
+      <c r="AN26" s="28"/>
+      <c r="AO26" s="28"/>
+      <c r="AP26" s="28"/>
+      <c r="AQ26" s="28"/>
+      <c r="AR26" s="28"/>
+      <c r="AS26" s="27"/>
+      <c r="AT26" s="28"/>
+      <c r="AU26" s="28"/>
+      <c r="AV26" s="28"/>
+      <c r="AW26" s="28"/>
+      <c r="AX26" s="28"/>
+      <c r="AY26" s="28"/>
+      <c r="AZ26" s="27"/>
+      <c r="BA26" s="28"/>
+      <c r="BB26" s="28"/>
+      <c r="BC26" s="28"/>
+      <c r="BD26" s="28"/>
+      <c r="BE26" s="28"/>
+      <c r="BF26" s="28"/>
+      <c r="BG26" s="27"/>
+      <c r="BH26" s="28"/>
+      <c r="BI26" s="28"/>
+      <c r="BJ26" s="28"/>
+      <c r="BK26" s="66"/>
+      <c r="BL26"/>
+      <c r="BM26"/>
+      <c r="BN26"/>
+      <c r="BO26"/>
+      <c r="BP26"/>
+      <c r="BQ26"/>
+      <c r="BR26"/>
+      <c r="BS26"/>
+      <c r="BT26"/>
+      <c r="BU26"/>
+      <c r="BV26"/>
+      <c r="BW26"/>
+      <c r="BX26"/>
+      <c r="BY26"/>
+      <c r="BZ26"/>
+      <c r="CA26"/>
+      <c r="CB26"/>
+      <c r="CC26"/>
+      <c r="CD26"/>
+      <c r="CE26"/>
+      <c r="CF26"/>
+      <c r="CG26"/>
+      <c r="CH26"/>
+      <c r="CI26"/>
+      <c r="CJ26"/>
+      <c r="CK26"/>
+      <c r="CL26"/>
+      <c r="CM26"/>
+      <c r="CN26"/>
+      <c r="CO26"/>
+      <c r="CP26"/>
+      <c r="CQ26"/>
+      <c r="CR26"/>
+      <c r="CS26"/>
+      <c r="CT26"/>
+      <c r="CU26"/>
+      <c r="CV26"/>
+      <c r="CW26"/>
+      <c r="CX26"/>
+      <c r="CY26"/>
+      <c r="CZ26"/>
+      <c r="DA26"/>
+      <c r="DB26"/>
+      <c r="DC26"/>
+      <c r="DD26"/>
+      <c r="DE26"/>
+      <c r="DF26"/>
+      <c r="DG26"/>
+      <c r="DH26"/>
+      <c r="DI26"/>
+      <c r="DJ26"/>
+      <c r="DK26"/>
+      <c r="DL26"/>
+      <c r="DM26"/>
+      <c r="DN26"/>
+      <c r="DO26"/>
+      <c r="DP26"/>
+      <c r="DQ26"/>
+      <c r="DR26"/>
+      <c r="DS26"/>
+      <c r="DT26"/>
+      <c r="DU26"/>
+      <c r="DV26"/>
+      <c r="DW26"/>
+      <c r="DX26"/>
+      <c r="DY26"/>
     </row>
-    <row r="25" spans="2:129" s="51" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="52"/>
-      <c r="C25" s="53" t="s">
+    <row r="27" spans="2:129" s="51" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B27" s="52"/>
+      <c r="C27" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="79"/>
-      <c r="E25" s="79"/>
-      <c r="F25" s="53" t="s">
+      <c r="D27" s="114"/>
+      <c r="E27" s="114"/>
+      <c r="F27" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="54">
+      <c r="G27" s="54">
         <v>45499</v>
       </c>
-      <c r="H25" s="55">
+      <c r="H27" s="55">
         <v>45499</v>
       </c>
-      <c r="I25" s="56">
+      <c r="I27" s="56">
         <v>0</v>
       </c>
-      <c r="J25" s="57"/>
-      <c r="K25" s="58"/>
-      <c r="L25" s="58"/>
-      <c r="M25" s="58"/>
-      <c r="N25" s="58"/>
-      <c r="O25" s="58"/>
-      <c r="P25" s="58"/>
-      <c r="Q25" s="57"/>
-      <c r="R25" s="58"/>
-      <c r="S25" s="58"/>
-      <c r="T25" s="58"/>
-      <c r="U25" s="58"/>
-      <c r="V25" s="58"/>
-      <c r="W25" s="58"/>
-      <c r="X25" s="57"/>
-      <c r="Y25" s="58"/>
-      <c r="Z25" s="58"/>
-      <c r="AA25" s="58"/>
-      <c r="AB25" s="58"/>
-      <c r="AC25" s="58"/>
-      <c r="AD25" s="59"/>
-      <c r="AE25" s="57"/>
-      <c r="AF25" s="58"/>
-      <c r="AG25" s="58"/>
-      <c r="AH25" s="58"/>
-      <c r="AI25" s="58"/>
-      <c r="AJ25" s="58"/>
-      <c r="AK25" s="59"/>
-      <c r="AL25" s="57"/>
-      <c r="AM25" s="58"/>
-      <c r="AN25" s="58"/>
-      <c r="AO25" s="58"/>
-      <c r="AP25" s="58"/>
-      <c r="AQ25" s="58"/>
-      <c r="AR25" s="59"/>
-      <c r="AS25" s="57"/>
-      <c r="AT25" s="58"/>
-      <c r="AU25" s="58"/>
-      <c r="AV25" s="58"/>
-      <c r="AW25" s="58"/>
-      <c r="AX25" s="58"/>
-      <c r="AY25" s="59"/>
-      <c r="AZ25" s="57"/>
-      <c r="BA25" s="58"/>
-      <c r="BB25" s="58"/>
-      <c r="BC25" s="58"/>
-      <c r="BD25" s="58"/>
-      <c r="BE25" s="58"/>
-      <c r="BF25" s="59"/>
-      <c r="BG25" s="57"/>
-      <c r="BH25" s="58"/>
-      <c r="BI25" s="58"/>
-      <c r="BJ25" s="58"/>
-      <c r="BK25" s="67"/>
-      <c r="BL25"/>
-      <c r="BM25"/>
-      <c r="BN25"/>
-      <c r="BO25"/>
-      <c r="BP25"/>
-      <c r="BQ25"/>
-      <c r="BR25"/>
-      <c r="BS25"/>
-      <c r="BT25"/>
-      <c r="BU25"/>
-      <c r="BV25"/>
-      <c r="BW25"/>
-      <c r="BX25"/>
-      <c r="BY25"/>
-      <c r="BZ25"/>
-      <c r="CA25"/>
-      <c r="CB25"/>
-      <c r="CC25"/>
-      <c r="CD25"/>
-      <c r="CE25"/>
-      <c r="CF25"/>
-      <c r="CG25"/>
-      <c r="CH25"/>
-      <c r="CI25"/>
-      <c r="CJ25"/>
-      <c r="CK25"/>
-      <c r="CL25"/>
-      <c r="CM25"/>
-      <c r="CN25"/>
-      <c r="CO25"/>
-      <c r="CP25"/>
-      <c r="CQ25"/>
-      <c r="CR25"/>
-      <c r="CS25"/>
-      <c r="CT25"/>
-      <c r="CU25"/>
-      <c r="CV25"/>
-      <c r="CW25"/>
-      <c r="CX25"/>
-      <c r="CY25"/>
-      <c r="CZ25"/>
-      <c r="DA25"/>
-      <c r="DB25"/>
-      <c r="DC25"/>
-      <c r="DD25"/>
-      <c r="DE25"/>
-      <c r="DF25"/>
-      <c r="DG25"/>
-      <c r="DH25"/>
-      <c r="DI25"/>
-      <c r="DJ25"/>
-      <c r="DK25"/>
-      <c r="DL25"/>
-      <c r="DM25"/>
-      <c r="DN25"/>
-      <c r="DO25"/>
-      <c r="DP25"/>
-      <c r="DQ25"/>
-      <c r="DR25"/>
-      <c r="DS25"/>
-      <c r="DT25"/>
-      <c r="DU25"/>
-      <c r="DV25"/>
-      <c r="DW25"/>
-      <c r="DX25"/>
-      <c r="DY25"/>
+      <c r="J27" s="57"/>
+      <c r="K27" s="58"/>
+      <c r="L27" s="58"/>
+      <c r="M27" s="58"/>
+      <c r="N27" s="58"/>
+      <c r="O27" s="58"/>
+      <c r="P27" s="58"/>
+      <c r="Q27" s="57"/>
+      <c r="R27" s="58"/>
+      <c r="S27" s="58"/>
+      <c r="T27" s="58"/>
+      <c r="U27" s="58"/>
+      <c r="V27" s="58"/>
+      <c r="W27" s="58"/>
+      <c r="X27" s="57"/>
+      <c r="Y27" s="58"/>
+      <c r="Z27" s="58"/>
+      <c r="AA27" s="58"/>
+      <c r="AB27" s="58"/>
+      <c r="AC27" s="58"/>
+      <c r="AD27" s="59"/>
+      <c r="AE27" s="57"/>
+      <c r="AF27" s="58"/>
+      <c r="AG27" s="58"/>
+      <c r="AH27" s="58"/>
+      <c r="AI27" s="58"/>
+      <c r="AJ27" s="58"/>
+      <c r="AK27" s="59"/>
+      <c r="AL27" s="57"/>
+      <c r="AM27" s="58"/>
+      <c r="AN27" s="58"/>
+      <c r="AO27" s="58"/>
+      <c r="AP27" s="58"/>
+      <c r="AQ27" s="58"/>
+      <c r="AR27" s="59"/>
+      <c r="AS27" s="57"/>
+      <c r="AT27" s="58"/>
+      <c r="AU27" s="58"/>
+      <c r="AV27" s="58"/>
+      <c r="AW27" s="58"/>
+      <c r="AX27" s="58"/>
+      <c r="AY27" s="59"/>
+      <c r="AZ27" s="57"/>
+      <c r="BA27" s="58"/>
+      <c r="BB27" s="58"/>
+      <c r="BC27" s="58"/>
+      <c r="BD27" s="58"/>
+      <c r="BE27" s="58"/>
+      <c r="BF27" s="59"/>
+      <c r="BG27" s="57"/>
+      <c r="BH27" s="58"/>
+      <c r="BI27" s="58"/>
+      <c r="BJ27" s="58"/>
+      <c r="BK27" s="67"/>
+      <c r="BL27"/>
+      <c r="BM27"/>
+      <c r="BN27"/>
+      <c r="BO27"/>
+      <c r="BP27"/>
+      <c r="BQ27"/>
+      <c r="BR27"/>
+      <c r="BS27"/>
+      <c r="BT27"/>
+      <c r="BU27"/>
+      <c r="BV27"/>
+      <c r="BW27"/>
+      <c r="BX27"/>
+      <c r="BY27"/>
+      <c r="BZ27"/>
+      <c r="CA27"/>
+      <c r="CB27"/>
+      <c r="CC27"/>
+      <c r="CD27"/>
+      <c r="CE27"/>
+      <c r="CF27"/>
+      <c r="CG27"/>
+      <c r="CH27"/>
+      <c r="CI27"/>
+      <c r="CJ27"/>
+      <c r="CK27"/>
+      <c r="CL27"/>
+      <c r="CM27"/>
+      <c r="CN27"/>
+      <c r="CO27"/>
+      <c r="CP27"/>
+      <c r="CQ27"/>
+      <c r="CR27"/>
+      <c r="CS27"/>
+      <c r="CT27"/>
+      <c r="CU27"/>
+      <c r="CV27"/>
+      <c r="CW27"/>
+      <c r="CX27"/>
+      <c r="CY27"/>
+      <c r="CZ27"/>
+      <c r="DA27"/>
+      <c r="DB27"/>
+      <c r="DC27"/>
+      <c r="DD27"/>
+      <c r="DE27"/>
+      <c r="DF27"/>
+      <c r="DG27"/>
+      <c r="DH27"/>
+      <c r="DI27"/>
+      <c r="DJ27"/>
+      <c r="DK27"/>
+      <c r="DL27"/>
+      <c r="DM27"/>
+      <c r="DN27"/>
+      <c r="DO27"/>
+      <c r="DP27"/>
+      <c r="DQ27"/>
+      <c r="DR27"/>
+      <c r="DS27"/>
+      <c r="DT27"/>
+      <c r="DU27"/>
+      <c r="DV27"/>
+      <c r="DW27"/>
+      <c r="DX27"/>
+      <c r="DY27"/>
     </row>
-    <row r="26" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="44" t="s">
+    <row r="28" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B28" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C28" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="80"/>
-      <c r="E26" s="81"/>
-      <c r="F26" s="16" t="s">
+      <c r="D28" s="87"/>
+      <c r="E28" s="88"/>
+      <c r="F28" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G26" s="50">
+      <c r="G28" s="50">
         <v>45500</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H28" s="3">
         <v>45501</v>
       </c>
-      <c r="I26" s="17">
-        <v>0</v>
-      </c>
-      <c r="J26" s="18"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19"/>
-      <c r="O26" s="19"/>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="19"/>
-      <c r="S26" s="19"/>
-      <c r="T26" s="19"/>
-      <c r="U26" s="19"/>
-      <c r="V26" s="19"/>
-      <c r="W26" s="19"/>
-      <c r="X26" s="18"/>
-      <c r="Y26" s="19"/>
-      <c r="Z26" s="19"/>
-      <c r="AA26" s="19"/>
-      <c r="AB26" s="19"/>
-      <c r="AC26" s="19"/>
-      <c r="AD26" s="20"/>
-      <c r="AE26" s="18"/>
-      <c r="AF26" s="19"/>
-      <c r="AG26" s="19"/>
-      <c r="AH26" s="19"/>
-      <c r="AI26" s="19"/>
-      <c r="AJ26" s="19"/>
-      <c r="AK26" s="20"/>
-      <c r="AL26" s="18"/>
-      <c r="AM26" s="19"/>
-      <c r="AN26" s="19"/>
-      <c r="AO26" s="19"/>
-      <c r="AP26" s="19"/>
-      <c r="AQ26" s="19"/>
-      <c r="AR26" s="20"/>
-      <c r="AS26" s="18"/>
-      <c r="AT26" s="19"/>
-      <c r="AU26" s="19"/>
-      <c r="AV26" s="19"/>
-      <c r="AW26" s="19"/>
-      <c r="AX26" s="19"/>
-      <c r="AY26" s="20"/>
-      <c r="AZ26" s="18"/>
-      <c r="BA26" s="19"/>
-      <c r="BB26" s="19"/>
-      <c r="BC26" s="19"/>
-      <c r="BD26" s="19"/>
-      <c r="BE26" s="19"/>
-      <c r="BF26" s="20"/>
-      <c r="BG26" s="18"/>
-      <c r="BH26" s="19"/>
-      <c r="BI26" s="19"/>
-      <c r="BJ26" s="19"/>
-      <c r="BK26" s="63"/>
-    </row>
-    <row r="27" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="14"/>
-      <c r="C27" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" s="92" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="92"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="74">
-        <v>45502</v>
-      </c>
-      <c r="H27" s="74">
-        <v>45527</v>
-      </c>
-      <c r="I27" s="17">
-        <v>0</v>
-      </c>
-      <c r="J27" s="23"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="21"/>
-      <c r="N27" s="21"/>
-      <c r="O27" s="21"/>
-      <c r="P27" s="21"/>
-      <c r="Q27" s="23"/>
-      <c r="R27" s="21"/>
-      <c r="S27" s="21"/>
-      <c r="T27" s="21"/>
-      <c r="U27" s="21"/>
-      <c r="V27" s="21"/>
-      <c r="W27" s="21"/>
-      <c r="X27" s="18"/>
-      <c r="Y27" s="19"/>
-      <c r="Z27" s="19"/>
-      <c r="AA27" s="19"/>
-      <c r="AB27" s="19"/>
-      <c r="AC27" s="19"/>
-      <c r="AD27" s="19"/>
-      <c r="AE27" s="18"/>
-      <c r="AF27" s="19"/>
-      <c r="AG27" s="19"/>
-      <c r="AH27" s="19"/>
-      <c r="AI27" s="19"/>
-      <c r="AJ27" s="19"/>
-      <c r="AK27" s="19"/>
-      <c r="AL27" s="18"/>
-      <c r="AM27" s="19"/>
-      <c r="AN27" s="19"/>
-      <c r="AO27" s="19"/>
-      <c r="AP27" s="19"/>
-      <c r="AQ27" s="19"/>
-      <c r="AR27" s="19"/>
-      <c r="AS27" s="18"/>
-      <c r="AT27" s="19"/>
-      <c r="AU27" s="19"/>
-      <c r="AV27" s="19"/>
-      <c r="AW27" s="19"/>
-      <c r="AX27" s="19"/>
-      <c r="AY27" s="19"/>
-      <c r="AZ27" s="18"/>
-      <c r="BA27" s="19"/>
-      <c r="BB27" s="19"/>
-      <c r="BC27" s="19"/>
-      <c r="BD27" s="19"/>
-      <c r="BE27" s="19"/>
-      <c r="BF27" s="19"/>
-      <c r="BG27" s="18"/>
-      <c r="BH27" s="19"/>
-      <c r="BI27" s="19"/>
-      <c r="BJ27" s="19"/>
-      <c r="BK27" s="63"/>
-    </row>
-    <row r="28" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="14"/>
-      <c r="C28" s="72"/>
-      <c r="D28" s="92" t="s">
-        <v>45</v>
-      </c>
-      <c r="E28" s="92"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="75"/>
-      <c r="H28" s="75"/>
       <c r="I28" s="17">
         <v>0</v>
       </c>
-      <c r="J28" s="23"/>
-      <c r="K28" s="21"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="21"/>
-      <c r="N28" s="21"/>
-      <c r="O28" s="21"/>
-      <c r="P28" s="21"/>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="21"/>
-      <c r="S28" s="21"/>
-      <c r="T28" s="21"/>
-      <c r="U28" s="21"/>
-      <c r="V28" s="21"/>
-      <c r="W28" s="21"/>
-      <c r="X28" s="23"/>
-      <c r="Y28" s="21"/>
-      <c r="Z28" s="21"/>
-      <c r="AA28" s="21"/>
-      <c r="AB28" s="21"/>
-      <c r="AC28" s="21"/>
-      <c r="AD28" s="21"/>
-      <c r="AE28" s="23"/>
-      <c r="AF28" s="21"/>
-      <c r="AG28" s="21"/>
-      <c r="AH28" s="21"/>
-      <c r="AI28" s="21"/>
-      <c r="AJ28" s="21"/>
-      <c r="AK28" s="21"/>
-      <c r="AL28" s="23"/>
-      <c r="AM28" s="21"/>
-      <c r="AN28" s="21"/>
-      <c r="AO28" s="21"/>
-      <c r="AP28" s="21"/>
-      <c r="AQ28" s="21"/>
-      <c r="AR28" s="21"/>
-      <c r="AS28" s="23"/>
-      <c r="AT28" s="21"/>
-      <c r="AU28" s="21"/>
-      <c r="AV28" s="21"/>
-      <c r="AW28" s="21"/>
-      <c r="AX28" s="21"/>
-      <c r="AY28" s="21"/>
-      <c r="AZ28" s="23"/>
-      <c r="BA28" s="21"/>
-      <c r="BB28" s="21"/>
-      <c r="BC28" s="21"/>
-      <c r="BD28" s="21"/>
-      <c r="BE28" s="21"/>
-      <c r="BF28" s="21"/>
-      <c r="BG28" s="23"/>
-      <c r="BH28" s="21"/>
-      <c r="BI28" s="21"/>
-      <c r="BJ28" s="21"/>
-      <c r="BK28" s="61"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+      <c r="V28" s="19"/>
+      <c r="W28" s="19"/>
+      <c r="X28" s="18"/>
+      <c r="Y28" s="19"/>
+      <c r="Z28" s="19"/>
+      <c r="AA28" s="19"/>
+      <c r="AB28" s="19"/>
+      <c r="AC28" s="19"/>
+      <c r="AD28" s="20"/>
+      <c r="AE28" s="18"/>
+      <c r="AF28" s="19"/>
+      <c r="AG28" s="19"/>
+      <c r="AH28" s="19"/>
+      <c r="AI28" s="19"/>
+      <c r="AJ28" s="19"/>
+      <c r="AK28" s="20"/>
+      <c r="AL28" s="18"/>
+      <c r="AM28" s="19"/>
+      <c r="AN28" s="19"/>
+      <c r="AO28" s="19"/>
+      <c r="AP28" s="19"/>
+      <c r="AQ28" s="19"/>
+      <c r="AR28" s="20"/>
+      <c r="AS28" s="18"/>
+      <c r="AT28" s="19"/>
+      <c r="AU28" s="19"/>
+      <c r="AV28" s="19"/>
+      <c r="AW28" s="19"/>
+      <c r="AX28" s="19"/>
+      <c r="AY28" s="20"/>
+      <c r="AZ28" s="18"/>
+      <c r="BA28" s="19"/>
+      <c r="BB28" s="19"/>
+      <c r="BC28" s="19"/>
+      <c r="BD28" s="19"/>
+      <c r="BE28" s="19"/>
+      <c r="BF28" s="20"/>
+      <c r="BG28" s="18"/>
+      <c r="BH28" s="19"/>
+      <c r="BI28" s="19"/>
+      <c r="BJ28" s="19"/>
+      <c r="BK28" s="63"/>
     </row>
-    <row r="29" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B29" s="14"/>
-      <c r="C29" s="72"/>
-      <c r="D29" s="92" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" s="92"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="75"/>
-      <c r="H29" s="75"/>
+      <c r="C29" s="112" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" s="83"/>
+      <c r="F29" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" s="97">
+        <v>45502</v>
+      </c>
+      <c r="H29" s="97">
+        <v>45527</v>
+      </c>
       <c r="I29" s="17">
         <v>0</v>
       </c>
@@ -4477,57 +4677,59 @@
       <c r="U29" s="21"/>
       <c r="V29" s="21"/>
       <c r="W29" s="21"/>
-      <c r="X29" s="23"/>
-      <c r="Y29" s="21"/>
-      <c r="Z29" s="21"/>
-      <c r="AA29" s="21"/>
-      <c r="AB29" s="21"/>
-      <c r="AC29" s="21"/>
-      <c r="AD29" s="21"/>
-      <c r="AE29" s="23"/>
-      <c r="AF29" s="21"/>
-      <c r="AG29" s="21"/>
-      <c r="AH29" s="21"/>
-      <c r="AI29" s="21"/>
-      <c r="AJ29" s="21"/>
-      <c r="AK29" s="21"/>
-      <c r="AL29" s="23"/>
-      <c r="AM29" s="21"/>
-      <c r="AN29" s="21"/>
-      <c r="AO29" s="21"/>
-      <c r="AP29" s="21"/>
-      <c r="AQ29" s="21"/>
-      <c r="AR29" s="21"/>
-      <c r="AS29" s="23"/>
-      <c r="AT29" s="21"/>
-      <c r="AU29" s="21"/>
-      <c r="AV29" s="21"/>
-      <c r="AW29" s="21"/>
-      <c r="AX29" s="21"/>
-      <c r="AY29" s="21"/>
-      <c r="AZ29" s="23"/>
-      <c r="BA29" s="21"/>
-      <c r="BB29" s="21"/>
-      <c r="BC29" s="21"/>
-      <c r="BD29" s="21"/>
-      <c r="BE29" s="21"/>
-      <c r="BF29" s="21"/>
-      <c r="BG29" s="23"/>
-      <c r="BH29" s="21"/>
-      <c r="BI29" s="21"/>
-      <c r="BJ29" s="21"/>
-      <c r="BK29" s="61"/>
+      <c r="X29" s="18"/>
+      <c r="Y29" s="19"/>
+      <c r="Z29" s="19"/>
+      <c r="AA29" s="19"/>
+      <c r="AB29" s="19"/>
+      <c r="AC29" s="19"/>
+      <c r="AD29" s="19"/>
+      <c r="AE29" s="18"/>
+      <c r="AF29" s="19"/>
+      <c r="AG29" s="19"/>
+      <c r="AH29" s="19"/>
+      <c r="AI29" s="19"/>
+      <c r="AJ29" s="19"/>
+      <c r="AK29" s="19"/>
+      <c r="AL29" s="18"/>
+      <c r="AM29" s="19"/>
+      <c r="AN29" s="19"/>
+      <c r="AO29" s="19"/>
+      <c r="AP29" s="19"/>
+      <c r="AQ29" s="19"/>
+      <c r="AR29" s="19"/>
+      <c r="AS29" s="18"/>
+      <c r="AT29" s="19"/>
+      <c r="AU29" s="19"/>
+      <c r="AV29" s="19"/>
+      <c r="AW29" s="19"/>
+      <c r="AX29" s="19"/>
+      <c r="AY29" s="19"/>
+      <c r="AZ29" s="18"/>
+      <c r="BA29" s="19"/>
+      <c r="BB29" s="19"/>
+      <c r="BC29" s="19"/>
+      <c r="BD29" s="19"/>
+      <c r="BE29" s="19"/>
+      <c r="BF29" s="19"/>
+      <c r="BG29" s="18"/>
+      <c r="BH29" s="19"/>
+      <c r="BI29" s="19"/>
+      <c r="BJ29" s="19"/>
+      <c r="BK29" s="63"/>
     </row>
-    <row r="30" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B30" s="14"/>
-      <c r="C30" s="72"/>
-      <c r="D30" s="101" t="s">
-        <v>47</v>
-      </c>
-      <c r="E30" s="101"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="75"/>
-      <c r="H30" s="75"/>
+      <c r="C30" s="95"/>
+      <c r="D30" s="83" t="s">
+        <v>45</v>
+      </c>
+      <c r="E30" s="83"/>
+      <c r="F30" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" s="98"/>
+      <c r="H30" s="98"/>
       <c r="I30" s="17">
         <v>0</v>
       </c>
@@ -4586,905 +4788,1204 @@
       <c r="BJ30" s="21"/>
       <c r="BK30" s="61"/>
     </row>
-    <row r="31" spans="2:129" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="30"/>
-      <c r="C31" s="73"/>
-      <c r="D31" s="102" t="s">
-        <v>48</v>
-      </c>
-      <c r="E31" s="102"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="76"/>
-      <c r="H31" s="76"/>
-      <c r="I31" s="47">
+    <row r="31" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B31" s="14"/>
+      <c r="C31" s="95"/>
+      <c r="D31" s="83" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="83"/>
+      <c r="F31" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="G31" s="98"/>
+      <c r="H31" s="98"/>
+      <c r="I31" s="17">
         <v>0</v>
       </c>
-      <c r="J31" s="27"/>
-      <c r="K31" s="28"/>
-      <c r="L31" s="28"/>
-      <c r="M31" s="28"/>
-      <c r="N31" s="28"/>
-      <c r="O31" s="28"/>
-      <c r="P31" s="28"/>
-      <c r="Q31" s="27"/>
-      <c r="R31" s="28"/>
-      <c r="S31" s="28"/>
-      <c r="T31" s="28"/>
-      <c r="U31" s="28"/>
-      <c r="V31" s="28"/>
-      <c r="W31" s="28"/>
-      <c r="X31" s="27"/>
-      <c r="Y31" s="28"/>
-      <c r="Z31" s="28"/>
-      <c r="AA31" s="28"/>
-      <c r="AB31" s="28"/>
-      <c r="AC31" s="28"/>
-      <c r="AD31" s="28"/>
-      <c r="AE31" s="27"/>
-      <c r="AF31" s="28"/>
-      <c r="AG31" s="28"/>
-      <c r="AH31" s="28"/>
-      <c r="AI31" s="28"/>
-      <c r="AJ31" s="28"/>
-      <c r="AK31" s="28"/>
-      <c r="AL31" s="27"/>
-      <c r="AM31" s="28"/>
-      <c r="AN31" s="28"/>
-      <c r="AO31" s="28"/>
-      <c r="AP31" s="28"/>
-      <c r="AQ31" s="28"/>
-      <c r="AR31" s="28"/>
-      <c r="AS31" s="27"/>
-      <c r="AT31" s="28"/>
-      <c r="AU31" s="28"/>
-      <c r="AV31" s="28"/>
-      <c r="AW31" s="28"/>
-      <c r="AX31" s="28"/>
-      <c r="AY31" s="28"/>
-      <c r="AZ31" s="27"/>
-      <c r="BA31" s="28"/>
-      <c r="BB31" s="28"/>
-      <c r="BC31" s="28"/>
-      <c r="BD31" s="28"/>
-      <c r="BE31" s="28"/>
-      <c r="BF31" s="28"/>
-      <c r="BG31" s="27"/>
-      <c r="BH31" s="28"/>
-      <c r="BI31" s="28"/>
-      <c r="BJ31" s="28"/>
-      <c r="BK31" s="66"/>
-      <c r="BL31"/>
-      <c r="BM31"/>
-      <c r="BN31"/>
-      <c r="BO31"/>
-      <c r="BP31"/>
-      <c r="BQ31"/>
-      <c r="BR31"/>
-      <c r="BS31"/>
-      <c r="BT31"/>
-      <c r="BU31"/>
-      <c r="BV31"/>
-      <c r="BW31"/>
-      <c r="BX31"/>
-      <c r="BY31"/>
-      <c r="BZ31"/>
-      <c r="CA31"/>
-      <c r="CB31"/>
-      <c r="CC31"/>
-      <c r="CD31"/>
-      <c r="CE31"/>
-      <c r="CF31"/>
-      <c r="CG31"/>
-      <c r="CH31"/>
-      <c r="CI31"/>
-      <c r="CJ31"/>
-      <c r="CK31"/>
-      <c r="CL31"/>
-      <c r="CM31"/>
-      <c r="CN31"/>
-      <c r="CO31"/>
-      <c r="CP31"/>
-      <c r="CQ31"/>
-      <c r="CR31"/>
-      <c r="CS31"/>
-      <c r="CT31"/>
-      <c r="CU31"/>
-      <c r="CV31"/>
-      <c r="CW31"/>
-      <c r="CX31"/>
-      <c r="CY31"/>
-      <c r="CZ31"/>
-      <c r="DA31"/>
-      <c r="DB31"/>
-      <c r="DC31"/>
-      <c r="DD31"/>
-      <c r="DE31"/>
-      <c r="DF31"/>
-      <c r="DG31"/>
-      <c r="DH31"/>
-      <c r="DI31"/>
-      <c r="DJ31"/>
-      <c r="DK31"/>
-      <c r="DL31"/>
-      <c r="DM31"/>
-      <c r="DN31"/>
-      <c r="DO31"/>
-      <c r="DP31"/>
-      <c r="DQ31"/>
-      <c r="DR31"/>
-      <c r="DS31"/>
-      <c r="DT31"/>
-      <c r="DU31"/>
-      <c r="DV31"/>
-      <c r="DW31"/>
-      <c r="DX31"/>
-      <c r="DY31"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="23"/>
+      <c r="R31" s="21"/>
+      <c r="S31" s="21"/>
+      <c r="T31" s="21"/>
+      <c r="U31" s="21"/>
+      <c r="V31" s="21"/>
+      <c r="W31" s="21"/>
+      <c r="X31" s="23"/>
+      <c r="Y31" s="21"/>
+      <c r="Z31" s="21"/>
+      <c r="AA31" s="21"/>
+      <c r="AB31" s="21"/>
+      <c r="AC31" s="21"/>
+      <c r="AD31" s="21"/>
+      <c r="AE31" s="23"/>
+      <c r="AF31" s="21"/>
+      <c r="AG31" s="21"/>
+      <c r="AH31" s="21"/>
+      <c r="AI31" s="21"/>
+      <c r="AJ31" s="21"/>
+      <c r="AK31" s="21"/>
+      <c r="AL31" s="23"/>
+      <c r="AM31" s="21"/>
+      <c r="AN31" s="21"/>
+      <c r="AO31" s="21"/>
+      <c r="AP31" s="21"/>
+      <c r="AQ31" s="21"/>
+      <c r="AR31" s="21"/>
+      <c r="AS31" s="23"/>
+      <c r="AT31" s="21"/>
+      <c r="AU31" s="21"/>
+      <c r="AV31" s="21"/>
+      <c r="AW31" s="21"/>
+      <c r="AX31" s="21"/>
+      <c r="AY31" s="21"/>
+      <c r="AZ31" s="23"/>
+      <c r="BA31" s="21"/>
+      <c r="BB31" s="21"/>
+      <c r="BC31" s="21"/>
+      <c r="BD31" s="21"/>
+      <c r="BE31" s="21"/>
+      <c r="BF31" s="21"/>
+      <c r="BG31" s="23"/>
+      <c r="BH31" s="21"/>
+      <c r="BI31" s="21"/>
+      <c r="BJ31" s="21"/>
+      <c r="BK31" s="61"/>
     </row>
-    <row r="32" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="26"/>
-      <c r="C32" s="82" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="80" t="s">
-        <v>44</v>
-      </c>
-      <c r="E32" s="81"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="77">
-        <v>45502</v>
-      </c>
-      <c r="H32" s="77">
-        <v>45527</v>
-      </c>
+    <row r="32" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B32" s="14"/>
+      <c r="C32" s="95"/>
+      <c r="D32" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="84"/>
+      <c r="F32" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G32" s="98"/>
+      <c r="H32" s="98"/>
       <c r="I32" s="17">
         <v>0</v>
       </c>
-      <c r="J32" s="18"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="19"/>
-      <c r="P32" s="19"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="19"/>
-      <c r="S32" s="19"/>
-      <c r="T32" s="19"/>
-      <c r="U32" s="19"/>
-      <c r="V32" s="19"/>
-      <c r="W32" s="19"/>
-      <c r="X32" s="18"/>
-      <c r="Y32" s="19"/>
-      <c r="Z32" s="19"/>
-      <c r="AA32" s="19"/>
-      <c r="AB32" s="19"/>
-      <c r="AC32" s="19"/>
-      <c r="AD32" s="19"/>
-      <c r="AE32" s="18"/>
-      <c r="AF32" s="19"/>
-      <c r="AG32" s="19"/>
-      <c r="AH32" s="19"/>
-      <c r="AI32" s="19"/>
-      <c r="AJ32" s="19"/>
-      <c r="AK32" s="19"/>
-      <c r="AL32" s="18"/>
-      <c r="AM32" s="19"/>
-      <c r="AN32" s="19"/>
-      <c r="AO32" s="19"/>
-      <c r="AP32" s="19"/>
-      <c r="AQ32" s="19"/>
-      <c r="AR32" s="19"/>
-      <c r="AS32" s="18"/>
-      <c r="AT32" s="19"/>
-      <c r="AU32" s="19"/>
-      <c r="AV32" s="19"/>
-      <c r="AW32" s="19"/>
-      <c r="AX32" s="19"/>
-      <c r="AY32" s="19"/>
-      <c r="AZ32" s="18"/>
-      <c r="BA32" s="19"/>
-      <c r="BB32" s="19"/>
-      <c r="BC32" s="19"/>
-      <c r="BD32" s="19"/>
-      <c r="BE32" s="19"/>
-      <c r="BF32" s="19"/>
-      <c r="BG32" s="18"/>
-      <c r="BH32" s="19"/>
-      <c r="BI32" s="19"/>
-      <c r="BJ32" s="19"/>
-      <c r="BK32" s="63"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="21"/>
+      <c r="U32" s="21"/>
+      <c r="V32" s="21"/>
+      <c r="W32" s="21"/>
+      <c r="X32" s="23"/>
+      <c r="Y32" s="21"/>
+      <c r="Z32" s="21"/>
+      <c r="AA32" s="21"/>
+      <c r="AB32" s="21"/>
+      <c r="AC32" s="21"/>
+      <c r="AD32" s="21"/>
+      <c r="AE32" s="23"/>
+      <c r="AF32" s="21"/>
+      <c r="AG32" s="21"/>
+      <c r="AH32" s="21"/>
+      <c r="AI32" s="21"/>
+      <c r="AJ32" s="21"/>
+      <c r="AK32" s="21"/>
+      <c r="AL32" s="23"/>
+      <c r="AM32" s="21"/>
+      <c r="AN32" s="21"/>
+      <c r="AO32" s="21"/>
+      <c r="AP32" s="21"/>
+      <c r="AQ32" s="21"/>
+      <c r="AR32" s="21"/>
+      <c r="AS32" s="23"/>
+      <c r="AT32" s="21"/>
+      <c r="AU32" s="21"/>
+      <c r="AV32" s="21"/>
+      <c r="AW32" s="21"/>
+      <c r="AX32" s="21"/>
+      <c r="AY32" s="21"/>
+      <c r="AZ32" s="23"/>
+      <c r="BA32" s="21"/>
+      <c r="BB32" s="21"/>
+      <c r="BC32" s="21"/>
+      <c r="BD32" s="21"/>
+      <c r="BE32" s="21"/>
+      <c r="BF32" s="21"/>
+      <c r="BG32" s="23"/>
+      <c r="BH32" s="21"/>
+      <c r="BI32" s="21"/>
+      <c r="BJ32" s="21"/>
+      <c r="BK32" s="61"/>
     </row>
-    <row r="33" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="14"/>
-      <c r="C33" s="72"/>
-      <c r="D33" s="103" t="s">
-        <v>45</v>
-      </c>
-      <c r="E33" s="104"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="75"/>
-      <c r="H33" s="75"/>
+    <row r="33" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B33" s="119"/>
+      <c r="C33" s="95"/>
+      <c r="D33" s="84" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="84"/>
+      <c r="F33" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="98"/>
+      <c r="H33" s="98"/>
       <c r="I33" s="17">
         <v>0</v>
       </c>
-      <c r="J33" s="23"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="21"/>
-      <c r="N33" s="21"/>
-      <c r="O33" s="21"/>
-      <c r="P33" s="21"/>
-      <c r="Q33" s="23"/>
-      <c r="R33" s="21"/>
-      <c r="S33" s="21"/>
-      <c r="T33" s="21"/>
-      <c r="U33" s="21"/>
-      <c r="V33" s="21"/>
-      <c r="W33" s="21"/>
-      <c r="X33" s="23"/>
-      <c r="Y33" s="21"/>
-      <c r="Z33" s="21"/>
-      <c r="AA33" s="21"/>
-      <c r="AB33" s="21"/>
-      <c r="AC33" s="21"/>
-      <c r="AD33" s="21"/>
-      <c r="AE33" s="23"/>
-      <c r="AF33" s="21"/>
-      <c r="AG33" s="21"/>
-      <c r="AH33" s="21"/>
-      <c r="AI33" s="21"/>
-      <c r="AJ33" s="21"/>
-      <c r="AK33" s="21"/>
-      <c r="AL33" s="23"/>
-      <c r="AM33" s="21"/>
-      <c r="AN33" s="21"/>
-      <c r="AO33" s="21"/>
-      <c r="AP33" s="21"/>
-      <c r="AQ33" s="21"/>
-      <c r="AR33" s="21"/>
-      <c r="AS33" s="23"/>
-      <c r="AT33" s="21"/>
-      <c r="AU33" s="21"/>
-      <c r="AV33" s="21"/>
-      <c r="AW33" s="21"/>
-      <c r="AX33" s="21"/>
-      <c r="AY33" s="21"/>
-      <c r="AZ33" s="23"/>
-      <c r="BA33" s="21"/>
-      <c r="BB33" s="21"/>
-      <c r="BC33" s="21"/>
-      <c r="BD33" s="21"/>
-      <c r="BE33" s="21"/>
-      <c r="BF33" s="21"/>
-      <c r="BG33" s="23"/>
-      <c r="BH33" s="21"/>
-      <c r="BI33" s="21"/>
-      <c r="BJ33" s="21"/>
-      <c r="BK33" s="61"/>
+      <c r="J33" s="120"/>
+      <c r="K33" s="121"/>
+      <c r="L33" s="121"/>
+      <c r="M33" s="121"/>
+      <c r="N33" s="121"/>
+      <c r="O33" s="121"/>
+      <c r="P33" s="121"/>
+      <c r="Q33" s="120"/>
+      <c r="R33" s="121"/>
+      <c r="S33" s="121"/>
+      <c r="T33" s="121"/>
+      <c r="U33" s="121"/>
+      <c r="V33" s="121"/>
+      <c r="W33" s="121"/>
+      <c r="X33" s="120"/>
+      <c r="Y33" s="121"/>
+      <c r="Z33" s="121"/>
+      <c r="AA33" s="121"/>
+      <c r="AB33" s="121"/>
+      <c r="AC33" s="121"/>
+      <c r="AD33" s="121"/>
+      <c r="AE33" s="120"/>
+      <c r="AF33" s="121"/>
+      <c r="AG33" s="121"/>
+      <c r="AH33" s="121"/>
+      <c r="AI33" s="121"/>
+      <c r="AJ33" s="121"/>
+      <c r="AK33" s="121"/>
+      <c r="AL33" s="120"/>
+      <c r="AM33" s="121"/>
+      <c r="AN33" s="121"/>
+      <c r="AO33" s="121"/>
+      <c r="AP33" s="121"/>
+      <c r="AQ33" s="121"/>
+      <c r="AR33" s="121"/>
+      <c r="AS33" s="120"/>
+      <c r="AT33" s="121"/>
+      <c r="AU33" s="121"/>
+      <c r="AV33" s="121"/>
+      <c r="AW33" s="121"/>
+      <c r="AX33" s="121"/>
+      <c r="AY33" s="121"/>
+      <c r="AZ33" s="120"/>
+      <c r="BA33" s="121"/>
+      <c r="BB33" s="121"/>
+      <c r="BC33" s="121"/>
+      <c r="BD33" s="121"/>
+      <c r="BE33" s="121"/>
+      <c r="BF33" s="121"/>
+      <c r="BG33" s="120"/>
+      <c r="BH33" s="121"/>
+      <c r="BI33" s="121"/>
+      <c r="BJ33" s="121"/>
+      <c r="BK33" s="122"/>
     </row>
-    <row r="34" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="14"/>
-      <c r="C34" s="72"/>
-      <c r="D34" s="103" t="s">
-        <v>46</v>
-      </c>
-      <c r="E34" s="104"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="75"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="17">
+    <row r="34" spans="2:129" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B34" s="30"/>
+      <c r="C34" s="85"/>
+      <c r="D34" s="86" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="86"/>
+      <c r="F34" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="G34" s="99"/>
+      <c r="H34" s="99"/>
+      <c r="I34" s="47">
         <v>0</v>
       </c>
-      <c r="J34" s="23"/>
-      <c r="K34" s="21"/>
-      <c r="L34" s="21"/>
-      <c r="M34" s="21"/>
-      <c r="N34" s="21"/>
-      <c r="O34" s="21"/>
-      <c r="P34" s="21"/>
-      <c r="Q34" s="23"/>
-      <c r="R34" s="21"/>
-      <c r="S34" s="21"/>
-      <c r="T34" s="21"/>
-      <c r="U34" s="21"/>
-      <c r="V34" s="21"/>
-      <c r="W34" s="21"/>
-      <c r="X34" s="23"/>
-      <c r="Y34" s="21"/>
-      <c r="Z34" s="21"/>
-      <c r="AA34" s="21"/>
-      <c r="AB34" s="21"/>
-      <c r="AC34" s="21"/>
-      <c r="AD34" s="21"/>
-      <c r="AE34" s="23"/>
-      <c r="AF34" s="21"/>
-      <c r="AG34" s="21"/>
-      <c r="AH34" s="21"/>
-      <c r="AI34" s="21"/>
-      <c r="AJ34" s="21"/>
-      <c r="AK34" s="21"/>
-      <c r="AL34" s="23"/>
-      <c r="AM34" s="21"/>
-      <c r="AN34" s="21"/>
-      <c r="AO34" s="21"/>
-      <c r="AP34" s="21"/>
-      <c r="AQ34" s="21"/>
-      <c r="AR34" s="21"/>
-      <c r="AS34" s="23"/>
-      <c r="AT34" s="21"/>
-      <c r="AU34" s="21"/>
-      <c r="AV34" s="21"/>
-      <c r="AW34" s="21"/>
-      <c r="AX34" s="21"/>
-      <c r="AY34" s="21"/>
-      <c r="AZ34" s="23"/>
-      <c r="BA34" s="21"/>
-      <c r="BB34" s="21"/>
-      <c r="BC34" s="21"/>
-      <c r="BD34" s="21"/>
-      <c r="BE34" s="21"/>
-      <c r="BF34" s="21"/>
-      <c r="BG34" s="23"/>
-      <c r="BH34" s="21"/>
-      <c r="BI34" s="21"/>
-      <c r="BJ34" s="21"/>
-      <c r="BK34" s="61"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="28"/>
+      <c r="N34" s="28"/>
+      <c r="O34" s="28"/>
+      <c r="P34" s="28"/>
+      <c r="Q34" s="27"/>
+      <c r="R34" s="28"/>
+      <c r="S34" s="28"/>
+      <c r="T34" s="28"/>
+      <c r="U34" s="28"/>
+      <c r="V34" s="28"/>
+      <c r="W34" s="28"/>
+      <c r="X34" s="27"/>
+      <c r="Y34" s="28"/>
+      <c r="Z34" s="28"/>
+      <c r="AA34" s="28"/>
+      <c r="AB34" s="28"/>
+      <c r="AC34" s="28"/>
+      <c r="AD34" s="28"/>
+      <c r="AE34" s="27"/>
+      <c r="AF34" s="28"/>
+      <c r="AG34" s="28"/>
+      <c r="AH34" s="28"/>
+      <c r="AI34" s="28"/>
+      <c r="AJ34" s="28"/>
+      <c r="AK34" s="28"/>
+      <c r="AL34" s="27"/>
+      <c r="AM34" s="28"/>
+      <c r="AN34" s="28"/>
+      <c r="AO34" s="28"/>
+      <c r="AP34" s="28"/>
+      <c r="AQ34" s="28"/>
+      <c r="AR34" s="28"/>
+      <c r="AS34" s="27"/>
+      <c r="AT34" s="28"/>
+      <c r="AU34" s="28"/>
+      <c r="AV34" s="28"/>
+      <c r="AW34" s="28"/>
+      <c r="AX34" s="28"/>
+      <c r="AY34" s="28"/>
+      <c r="AZ34" s="27"/>
+      <c r="BA34" s="28"/>
+      <c r="BB34" s="28"/>
+      <c r="BC34" s="28"/>
+      <c r="BD34" s="28"/>
+      <c r="BE34" s="28"/>
+      <c r="BF34" s="28"/>
+      <c r="BG34" s="27"/>
+      <c r="BH34" s="28"/>
+      <c r="BI34" s="28"/>
+      <c r="BJ34" s="28"/>
+      <c r="BK34" s="66"/>
+      <c r="BL34"/>
+      <c r="BM34"/>
+      <c r="BN34"/>
+      <c r="BO34"/>
+      <c r="BP34"/>
+      <c r="BQ34"/>
+      <c r="BR34"/>
+      <c r="BS34"/>
+      <c r="BT34"/>
+      <c r="BU34"/>
+      <c r="BV34"/>
+      <c r="BW34"/>
+      <c r="BX34"/>
+      <c r="BY34"/>
+      <c r="BZ34"/>
+      <c r="CA34"/>
+      <c r="CB34"/>
+      <c r="CC34"/>
+      <c r="CD34"/>
+      <c r="CE34"/>
+      <c r="CF34"/>
+      <c r="CG34"/>
+      <c r="CH34"/>
+      <c r="CI34"/>
+      <c r="CJ34"/>
+      <c r="CK34"/>
+      <c r="CL34"/>
+      <c r="CM34"/>
+      <c r="CN34"/>
+      <c r="CO34"/>
+      <c r="CP34"/>
+      <c r="CQ34"/>
+      <c r="CR34"/>
+      <c r="CS34"/>
+      <c r="CT34"/>
+      <c r="CU34"/>
+      <c r="CV34"/>
+      <c r="CW34"/>
+      <c r="CX34"/>
+      <c r="CY34"/>
+      <c r="CZ34"/>
+      <c r="DA34"/>
+      <c r="DB34"/>
+      <c r="DC34"/>
+      <c r="DD34"/>
+      <c r="DE34"/>
+      <c r="DF34"/>
+      <c r="DG34"/>
+      <c r="DH34"/>
+      <c r="DI34"/>
+      <c r="DJ34"/>
+      <c r="DK34"/>
+      <c r="DL34"/>
+      <c r="DM34"/>
+      <c r="DN34"/>
+      <c r="DO34"/>
+      <c r="DP34"/>
+      <c r="DQ34"/>
+      <c r="DR34"/>
+      <c r="DS34"/>
+      <c r="DT34"/>
+      <c r="DU34"/>
+      <c r="DV34"/>
+      <c r="DW34"/>
+      <c r="DX34"/>
+      <c r="DY34"/>
     </row>
-    <row r="35" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="14"/>
-      <c r="C35" s="72"/>
-      <c r="D35" s="103" t="s">
-        <v>47</v>
-      </c>
-      <c r="E35" s="104"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="75"/>
-      <c r="H35" s="75"/>
+    <row r="35" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B35" s="26"/>
+      <c r="C35" s="94" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="87" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="88"/>
+      <c r="F35" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G35" s="106">
+        <v>45502</v>
+      </c>
+      <c r="H35" s="106">
+        <v>45527</v>
+      </c>
       <c r="I35" s="17">
         <v>0</v>
       </c>
-      <c r="J35" s="23"/>
-      <c r="K35" s="21"/>
-      <c r="L35" s="21"/>
-      <c r="M35" s="21"/>
-      <c r="N35" s="21"/>
-      <c r="O35" s="21"/>
-      <c r="P35" s="21"/>
-      <c r="Q35" s="23"/>
-      <c r="R35" s="21"/>
-      <c r="S35" s="21"/>
-      <c r="T35" s="21"/>
-      <c r="U35" s="21"/>
-      <c r="V35" s="21"/>
-      <c r="W35" s="21"/>
-      <c r="X35" s="23"/>
-      <c r="Y35" s="21"/>
-      <c r="Z35" s="21"/>
-      <c r="AA35" s="21"/>
-      <c r="AB35" s="21"/>
-      <c r="AC35" s="21"/>
-      <c r="AD35" s="21"/>
-      <c r="AE35" s="23"/>
-      <c r="AF35" s="21"/>
-      <c r="AG35" s="21"/>
-      <c r="AH35" s="21"/>
-      <c r="AI35" s="21"/>
-      <c r="AJ35" s="21"/>
-      <c r="AK35" s="21"/>
-      <c r="AL35" s="23"/>
-      <c r="AM35" s="21"/>
-      <c r="AN35" s="21"/>
-      <c r="AO35" s="21"/>
-      <c r="AP35" s="21"/>
-      <c r="AQ35" s="21"/>
-      <c r="AR35" s="21"/>
-      <c r="AS35" s="23"/>
-      <c r="AT35" s="21"/>
-      <c r="AU35" s="21"/>
-      <c r="AV35" s="21"/>
-      <c r="AW35" s="21"/>
-      <c r="AX35" s="21"/>
-      <c r="AY35" s="21"/>
-      <c r="AZ35" s="23"/>
-      <c r="BA35" s="21"/>
-      <c r="BB35" s="21"/>
-      <c r="BC35" s="21"/>
-      <c r="BD35" s="21"/>
-      <c r="BE35" s="21"/>
-      <c r="BF35" s="21"/>
-      <c r="BG35" s="23"/>
-      <c r="BH35" s="21"/>
-      <c r="BI35" s="21"/>
-      <c r="BJ35" s="21"/>
-      <c r="BK35" s="61"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="18"/>
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="19"/>
+      <c r="V35" s="19"/>
+      <c r="W35" s="19"/>
+      <c r="X35" s="18"/>
+      <c r="Y35" s="19"/>
+      <c r="Z35" s="19"/>
+      <c r="AA35" s="19"/>
+      <c r="AB35" s="19"/>
+      <c r="AC35" s="19"/>
+      <c r="AD35" s="19"/>
+      <c r="AE35" s="18"/>
+      <c r="AF35" s="19"/>
+      <c r="AG35" s="19"/>
+      <c r="AH35" s="19"/>
+      <c r="AI35" s="19"/>
+      <c r="AJ35" s="19"/>
+      <c r="AK35" s="19"/>
+      <c r="AL35" s="18"/>
+      <c r="AM35" s="19"/>
+      <c r="AN35" s="19"/>
+      <c r="AO35" s="19"/>
+      <c r="AP35" s="19"/>
+      <c r="AQ35" s="19"/>
+      <c r="AR35" s="19"/>
+      <c r="AS35" s="18"/>
+      <c r="AT35" s="19"/>
+      <c r="AU35" s="19"/>
+      <c r="AV35" s="19"/>
+      <c r="AW35" s="19"/>
+      <c r="AX35" s="19"/>
+      <c r="AY35" s="19"/>
+      <c r="AZ35" s="18"/>
+      <c r="BA35" s="19"/>
+      <c r="BB35" s="19"/>
+      <c r="BC35" s="19"/>
+      <c r="BD35" s="19"/>
+      <c r="BE35" s="19"/>
+      <c r="BF35" s="19"/>
+      <c r="BG35" s="18"/>
+      <c r="BH35" s="19"/>
+      <c r="BI35" s="19"/>
+      <c r="BJ35" s="19"/>
+      <c r="BK35" s="63"/>
     </row>
-    <row r="36" spans="2:129" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="15"/>
-      <c r="C36" s="83"/>
-      <c r="D36" s="105" t="s">
-        <v>48</v>
-      </c>
-      <c r="E36" s="106"/>
-      <c r="F36" s="37"/>
-      <c r="G36" s="78"/>
-      <c r="H36" s="78"/>
-      <c r="I36" s="36">
+    <row r="36" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B36" s="14"/>
+      <c r="C36" s="95"/>
+      <c r="D36" s="107" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" s="108"/>
+      <c r="F36" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="G36" s="98"/>
+      <c r="H36" s="98"/>
+      <c r="I36" s="17">
         <v>0</v>
       </c>
-      <c r="J36" s="24"/>
-      <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="25"/>
-      <c r="O36" s="25"/>
-      <c r="P36" s="25"/>
-      <c r="Q36" s="24"/>
-      <c r="R36" s="25"/>
-      <c r="S36" s="25"/>
-      <c r="T36" s="25"/>
-      <c r="U36" s="25"/>
-      <c r="V36" s="25"/>
-      <c r="W36" s="25"/>
-      <c r="X36" s="24"/>
-      <c r="Y36" s="25"/>
-      <c r="Z36" s="25"/>
-      <c r="AA36" s="25"/>
-      <c r="AB36" s="25"/>
-      <c r="AC36" s="25"/>
-      <c r="AD36" s="25"/>
-      <c r="AE36" s="24"/>
-      <c r="AF36" s="25"/>
-      <c r="AG36" s="25"/>
-      <c r="AH36" s="25"/>
-      <c r="AI36" s="25"/>
-      <c r="AJ36" s="25"/>
-      <c r="AK36" s="25"/>
-      <c r="AL36" s="24"/>
-      <c r="AM36" s="25"/>
-      <c r="AN36" s="25"/>
-      <c r="AO36" s="25"/>
-      <c r="AP36" s="25"/>
-      <c r="AQ36" s="25"/>
-      <c r="AR36" s="25"/>
-      <c r="AS36" s="24"/>
-      <c r="AT36" s="25"/>
-      <c r="AU36" s="25"/>
-      <c r="AV36" s="25"/>
-      <c r="AW36" s="25"/>
-      <c r="AX36" s="25"/>
-      <c r="AY36" s="25"/>
-      <c r="AZ36" s="24"/>
-      <c r="BA36" s="25"/>
-      <c r="BB36" s="25"/>
-      <c r="BC36" s="25"/>
-      <c r="BD36" s="25"/>
-      <c r="BE36" s="25"/>
-      <c r="BF36" s="25"/>
-      <c r="BG36" s="24"/>
-      <c r="BH36" s="25"/>
-      <c r="BI36" s="25"/>
-      <c r="BJ36" s="25"/>
-      <c r="BK36" s="62"/>
-      <c r="BL36"/>
-      <c r="BM36"/>
-      <c r="BN36"/>
-      <c r="BO36"/>
-      <c r="BP36"/>
-      <c r="BQ36"/>
-      <c r="BR36"/>
-      <c r="BS36"/>
-      <c r="BT36"/>
-      <c r="BU36"/>
-      <c r="BV36"/>
-      <c r="BW36"/>
-      <c r="BX36"/>
-      <c r="BY36"/>
-      <c r="BZ36"/>
-      <c r="CA36"/>
-      <c r="CB36"/>
-      <c r="CC36"/>
-      <c r="CD36"/>
-      <c r="CE36"/>
-      <c r="CF36"/>
-      <c r="CG36"/>
-      <c r="CH36"/>
-      <c r="CI36"/>
-      <c r="CJ36"/>
-      <c r="CK36"/>
-      <c r="CL36"/>
-      <c r="CM36"/>
-      <c r="CN36"/>
-      <c r="CO36"/>
-      <c r="CP36"/>
-      <c r="CQ36"/>
-      <c r="CR36"/>
-      <c r="CS36"/>
-      <c r="CT36"/>
-      <c r="CU36"/>
-      <c r="CV36"/>
-      <c r="CW36"/>
-      <c r="CX36"/>
-      <c r="CY36"/>
-      <c r="CZ36"/>
-      <c r="DA36"/>
-      <c r="DB36"/>
-      <c r="DC36"/>
-      <c r="DD36"/>
-      <c r="DE36"/>
-      <c r="DF36"/>
-      <c r="DG36"/>
-      <c r="DH36"/>
-      <c r="DI36"/>
-      <c r="DJ36"/>
-      <c r="DK36"/>
-      <c r="DL36"/>
-      <c r="DM36"/>
-      <c r="DN36"/>
-      <c r="DO36"/>
-      <c r="DP36"/>
-      <c r="DQ36"/>
-      <c r="DR36"/>
-      <c r="DS36"/>
-      <c r="DT36"/>
-      <c r="DU36"/>
-      <c r="DV36"/>
-      <c r="DW36"/>
-      <c r="DX36"/>
-      <c r="DY36"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="21"/>
+      <c r="O36" s="21"/>
+      <c r="P36" s="21"/>
+      <c r="Q36" s="23"/>
+      <c r="R36" s="21"/>
+      <c r="S36" s="21"/>
+      <c r="T36" s="21"/>
+      <c r="U36" s="21"/>
+      <c r="V36" s="21"/>
+      <c r="W36" s="21"/>
+      <c r="X36" s="23"/>
+      <c r="Y36" s="21"/>
+      <c r="Z36" s="21"/>
+      <c r="AA36" s="21"/>
+      <c r="AB36" s="21"/>
+      <c r="AC36" s="21"/>
+      <c r="AD36" s="21"/>
+      <c r="AE36" s="23"/>
+      <c r="AF36" s="21"/>
+      <c r="AG36" s="21"/>
+      <c r="AH36" s="21"/>
+      <c r="AI36" s="21"/>
+      <c r="AJ36" s="21"/>
+      <c r="AK36" s="21"/>
+      <c r="AL36" s="23"/>
+      <c r="AM36" s="21"/>
+      <c r="AN36" s="21"/>
+      <c r="AO36" s="21"/>
+      <c r="AP36" s="21"/>
+      <c r="AQ36" s="21"/>
+      <c r="AR36" s="21"/>
+      <c r="AS36" s="23"/>
+      <c r="AT36" s="21"/>
+      <c r="AU36" s="21"/>
+      <c r="AV36" s="21"/>
+      <c r="AW36" s="21"/>
+      <c r="AX36" s="21"/>
+      <c r="AY36" s="21"/>
+      <c r="AZ36" s="23"/>
+      <c r="BA36" s="21"/>
+      <c r="BB36" s="21"/>
+      <c r="BC36" s="21"/>
+      <c r="BD36" s="21"/>
+      <c r="BE36" s="21"/>
+      <c r="BF36" s="21"/>
+      <c r="BG36" s="23"/>
+      <c r="BH36" s="21"/>
+      <c r="BI36" s="21"/>
+      <c r="BJ36" s="21"/>
+      <c r="BK36" s="61"/>
     </row>
-    <row r="37" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D37" s="80" t="s">
-        <v>54</v>
-      </c>
-      <c r="E37" s="81"/>
+    <row r="37" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B37" s="14"/>
+      <c r="C37" s="95"/>
+      <c r="D37" s="107" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" s="108"/>
       <c r="F37" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="G37" s="50">
-        <v>45528</v>
-      </c>
-      <c r="H37" s="50">
-        <v>45540</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="G37" s="98"/>
+      <c r="H37" s="98"/>
       <c r="I37" s="17">
         <v>0</v>
       </c>
-      <c r="J37" s="18"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
-      <c r="P37" s="19"/>
-      <c r="Q37" s="18"/>
-      <c r="R37" s="19"/>
-      <c r="S37" s="19"/>
-      <c r="T37" s="19"/>
-      <c r="U37" s="19"/>
-      <c r="V37" s="19"/>
-      <c r="W37" s="19"/>
-      <c r="X37" s="18"/>
-      <c r="Y37" s="19"/>
-      <c r="Z37" s="19"/>
-      <c r="AA37" s="19"/>
-      <c r="AB37" s="19"/>
-      <c r="AC37" s="19"/>
-      <c r="AD37" s="19"/>
-      <c r="AE37" s="18"/>
-      <c r="AF37" s="19"/>
-      <c r="AG37" s="19"/>
-      <c r="AH37" s="19"/>
-      <c r="AI37" s="19"/>
-      <c r="AJ37" s="19"/>
-      <c r="AK37" s="19"/>
-      <c r="AL37" s="18"/>
-      <c r="AM37" s="19"/>
-      <c r="AN37" s="19"/>
-      <c r="AO37" s="19"/>
-      <c r="AP37" s="19"/>
-      <c r="AQ37" s="19"/>
-      <c r="AR37" s="19"/>
-      <c r="AS37" s="18"/>
-      <c r="AT37" s="19"/>
-      <c r="AU37" s="19"/>
-      <c r="AV37" s="19"/>
-      <c r="AW37" s="19"/>
-      <c r="AX37" s="19"/>
-      <c r="AY37" s="19"/>
-      <c r="AZ37" s="18"/>
-      <c r="BA37" s="19"/>
-      <c r="BB37" s="19"/>
-      <c r="BC37" s="19"/>
-      <c r="BD37" s="19"/>
-      <c r="BE37" s="19"/>
-      <c r="BF37" s="19"/>
-      <c r="BG37" s="18"/>
-      <c r="BH37" s="19"/>
-      <c r="BI37" s="19"/>
-      <c r="BJ37" s="19"/>
-      <c r="BK37" s="63"/>
+      <c r="J37" s="23"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="21"/>
+      <c r="O37" s="21"/>
+      <c r="P37" s="21"/>
+      <c r="Q37" s="23"/>
+      <c r="R37" s="21"/>
+      <c r="S37" s="21"/>
+      <c r="T37" s="21"/>
+      <c r="U37" s="21"/>
+      <c r="V37" s="21"/>
+      <c r="W37" s="21"/>
+      <c r="X37" s="23"/>
+      <c r="Y37" s="21"/>
+      <c r="Z37" s="21"/>
+      <c r="AA37" s="21"/>
+      <c r="AB37" s="21"/>
+      <c r="AC37" s="21"/>
+      <c r="AD37" s="21"/>
+      <c r="AE37" s="23"/>
+      <c r="AF37" s="21"/>
+      <c r="AG37" s="21"/>
+      <c r="AH37" s="21"/>
+      <c r="AI37" s="21"/>
+      <c r="AJ37" s="21"/>
+      <c r="AK37" s="21"/>
+      <c r="AL37" s="23"/>
+      <c r="AM37" s="21"/>
+      <c r="AN37" s="21"/>
+      <c r="AO37" s="21"/>
+      <c r="AP37" s="21"/>
+      <c r="AQ37" s="21"/>
+      <c r="AR37" s="21"/>
+      <c r="AS37" s="23"/>
+      <c r="AT37" s="21"/>
+      <c r="AU37" s="21"/>
+      <c r="AV37" s="21"/>
+      <c r="AW37" s="21"/>
+      <c r="AX37" s="21"/>
+      <c r="AY37" s="21"/>
+      <c r="AZ37" s="23"/>
+      <c r="BA37" s="21"/>
+      <c r="BB37" s="21"/>
+      <c r="BC37" s="21"/>
+      <c r="BD37" s="21"/>
+      <c r="BE37" s="21"/>
+      <c r="BF37" s="21"/>
+      <c r="BG37" s="23"/>
+      <c r="BH37" s="21"/>
+      <c r="BI37" s="21"/>
+      <c r="BJ37" s="21"/>
+      <c r="BK37" s="61"/>
     </row>
-    <row r="38" spans="2:129" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="15"/>
-      <c r="C38" s="5" t="s">
+    <row r="38" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B38" s="14"/>
+      <c r="C38" s="95"/>
+      <c r="D38" s="107" t="s">
+        <v>47</v>
+      </c>
+      <c r="E38" s="108"/>
+      <c r="F38" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G38" s="98"/>
+      <c r="H38" s="98"/>
+      <c r="I38" s="17">
+        <v>0</v>
+      </c>
+      <c r="J38" s="23"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="21"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="21"/>
+      <c r="P38" s="21"/>
+      <c r="Q38" s="23"/>
+      <c r="R38" s="21"/>
+      <c r="S38" s="21"/>
+      <c r="T38" s="21"/>
+      <c r="U38" s="21"/>
+      <c r="V38" s="21"/>
+      <c r="W38" s="21"/>
+      <c r="X38" s="23"/>
+      <c r="Y38" s="21"/>
+      <c r="Z38" s="21"/>
+      <c r="AA38" s="21"/>
+      <c r="AB38" s="21"/>
+      <c r="AC38" s="21"/>
+      <c r="AD38" s="21"/>
+      <c r="AE38" s="23"/>
+      <c r="AF38" s="21"/>
+      <c r="AG38" s="21"/>
+      <c r="AH38" s="21"/>
+      <c r="AI38" s="21"/>
+      <c r="AJ38" s="21"/>
+      <c r="AK38" s="21"/>
+      <c r="AL38" s="23"/>
+      <c r="AM38" s="21"/>
+      <c r="AN38" s="21"/>
+      <c r="AO38" s="21"/>
+      <c r="AP38" s="21"/>
+      <c r="AQ38" s="21"/>
+      <c r="AR38" s="21"/>
+      <c r="AS38" s="23"/>
+      <c r="AT38" s="21"/>
+      <c r="AU38" s="21"/>
+      <c r="AV38" s="21"/>
+      <c r="AW38" s="21"/>
+      <c r="AX38" s="21"/>
+      <c r="AY38" s="21"/>
+      <c r="AZ38" s="23"/>
+      <c r="BA38" s="21"/>
+      <c r="BB38" s="21"/>
+      <c r="BC38" s="21"/>
+      <c r="BD38" s="21"/>
+      <c r="BE38" s="21"/>
+      <c r="BF38" s="21"/>
+      <c r="BG38" s="23"/>
+      <c r="BH38" s="21"/>
+      <c r="BI38" s="21"/>
+      <c r="BJ38" s="21"/>
+      <c r="BK38" s="61"/>
+    </row>
+    <row r="39" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B39" s="119"/>
+      <c r="C39" s="95"/>
+      <c r="D39" s="107" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="108"/>
+      <c r="F39" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="98"/>
+      <c r="H39" s="98"/>
+      <c r="I39" s="17">
+        <v>0</v>
+      </c>
+      <c r="J39" s="120"/>
+      <c r="K39" s="121"/>
+      <c r="L39" s="121"/>
+      <c r="M39" s="121"/>
+      <c r="N39" s="121"/>
+      <c r="O39" s="121"/>
+      <c r="P39" s="121"/>
+      <c r="Q39" s="120"/>
+      <c r="R39" s="121"/>
+      <c r="S39" s="121"/>
+      <c r="T39" s="121"/>
+      <c r="U39" s="121"/>
+      <c r="V39" s="121"/>
+      <c r="W39" s="121"/>
+      <c r="X39" s="120"/>
+      <c r="Y39" s="121"/>
+      <c r="Z39" s="121"/>
+      <c r="AA39" s="121"/>
+      <c r="AB39" s="121"/>
+      <c r="AC39" s="121"/>
+      <c r="AD39" s="121"/>
+      <c r="AE39" s="120"/>
+      <c r="AF39" s="121"/>
+      <c r="AG39" s="121"/>
+      <c r="AH39" s="121"/>
+      <c r="AI39" s="121"/>
+      <c r="AJ39" s="121"/>
+      <c r="AK39" s="121"/>
+      <c r="AL39" s="120"/>
+      <c r="AM39" s="121"/>
+      <c r="AN39" s="121"/>
+      <c r="AO39" s="121"/>
+      <c r="AP39" s="121"/>
+      <c r="AQ39" s="121"/>
+      <c r="AR39" s="121"/>
+      <c r="AS39" s="120"/>
+      <c r="AT39" s="121"/>
+      <c r="AU39" s="121"/>
+      <c r="AV39" s="121"/>
+      <c r="AW39" s="121"/>
+      <c r="AX39" s="121"/>
+      <c r="AY39" s="121"/>
+      <c r="AZ39" s="120"/>
+      <c r="BA39" s="121"/>
+      <c r="BB39" s="121"/>
+      <c r="BC39" s="121"/>
+      <c r="BD39" s="121"/>
+      <c r="BE39" s="121"/>
+      <c r="BF39" s="121"/>
+      <c r="BG39" s="120"/>
+      <c r="BH39" s="121"/>
+      <c r="BI39" s="121"/>
+      <c r="BJ39" s="121"/>
+      <c r="BK39" s="122"/>
+    </row>
+    <row r="40" spans="2:129" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B40" s="15"/>
+      <c r="C40" s="96"/>
+      <c r="D40" s="109" t="s">
+        <v>48</v>
+      </c>
+      <c r="E40" s="110"/>
+      <c r="F40" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="G40" s="113"/>
+      <c r="H40" s="113"/>
+      <c r="I40" s="36">
+        <v>0</v>
+      </c>
+      <c r="J40" s="24"/>
+      <c r="K40" s="25"/>
+      <c r="L40" s="25"/>
+      <c r="M40" s="25"/>
+      <c r="N40" s="25"/>
+      <c r="O40" s="25"/>
+      <c r="P40" s="25"/>
+      <c r="Q40" s="24"/>
+      <c r="R40" s="25"/>
+      <c r="S40" s="25"/>
+      <c r="T40" s="25"/>
+      <c r="U40" s="25"/>
+      <c r="V40" s="25"/>
+      <c r="W40" s="25"/>
+      <c r="X40" s="24"/>
+      <c r="Y40" s="25"/>
+      <c r="Z40" s="25"/>
+      <c r="AA40" s="25"/>
+      <c r="AB40" s="25"/>
+      <c r="AC40" s="25"/>
+      <c r="AD40" s="25"/>
+      <c r="AE40" s="24"/>
+      <c r="AF40" s="25"/>
+      <c r="AG40" s="25"/>
+      <c r="AH40" s="25"/>
+      <c r="AI40" s="25"/>
+      <c r="AJ40" s="25"/>
+      <c r="AK40" s="25"/>
+      <c r="AL40" s="24"/>
+      <c r="AM40" s="25"/>
+      <c r="AN40" s="25"/>
+      <c r="AO40" s="25"/>
+      <c r="AP40" s="25"/>
+      <c r="AQ40" s="25"/>
+      <c r="AR40" s="25"/>
+      <c r="AS40" s="24"/>
+      <c r="AT40" s="25"/>
+      <c r="AU40" s="25"/>
+      <c r="AV40" s="25"/>
+      <c r="AW40" s="25"/>
+      <c r="AX40" s="25"/>
+      <c r="AY40" s="25"/>
+      <c r="AZ40" s="24"/>
+      <c r="BA40" s="25"/>
+      <c r="BB40" s="25"/>
+      <c r="BC40" s="25"/>
+      <c r="BD40" s="25"/>
+      <c r="BE40" s="25"/>
+      <c r="BF40" s="25"/>
+      <c r="BG40" s="24"/>
+      <c r="BH40" s="25"/>
+      <c r="BI40" s="25"/>
+      <c r="BJ40" s="25"/>
+      <c r="BK40" s="62"/>
+      <c r="BL40"/>
+      <c r="BM40"/>
+      <c r="BN40"/>
+      <c r="BO40"/>
+      <c r="BP40"/>
+      <c r="BQ40"/>
+      <c r="BR40"/>
+      <c r="BS40"/>
+      <c r="BT40"/>
+      <c r="BU40"/>
+      <c r="BV40"/>
+      <c r="BW40"/>
+      <c r="BX40"/>
+      <c r="BY40"/>
+      <c r="BZ40"/>
+      <c r="CA40"/>
+      <c r="CB40"/>
+      <c r="CC40"/>
+      <c r="CD40"/>
+      <c r="CE40"/>
+      <c r="CF40"/>
+      <c r="CG40"/>
+      <c r="CH40"/>
+      <c r="CI40"/>
+      <c r="CJ40"/>
+      <c r="CK40"/>
+      <c r="CL40"/>
+      <c r="CM40"/>
+      <c r="CN40"/>
+      <c r="CO40"/>
+      <c r="CP40"/>
+      <c r="CQ40"/>
+      <c r="CR40"/>
+      <c r="CS40"/>
+      <c r="CT40"/>
+      <c r="CU40"/>
+      <c r="CV40"/>
+      <c r="CW40"/>
+      <c r="CX40"/>
+      <c r="CY40"/>
+      <c r="CZ40"/>
+      <c r="DA40"/>
+      <c r="DB40"/>
+      <c r="DC40"/>
+      <c r="DD40"/>
+      <c r="DE40"/>
+      <c r="DF40"/>
+      <c r="DG40"/>
+      <c r="DH40"/>
+      <c r="DI40"/>
+      <c r="DJ40"/>
+      <c r="DK40"/>
+      <c r="DL40"/>
+      <c r="DM40"/>
+      <c r="DN40"/>
+      <c r="DO40"/>
+      <c r="DP40"/>
+      <c r="DQ40"/>
+      <c r="DR40"/>
+      <c r="DS40"/>
+      <c r="DT40"/>
+      <c r="DU40"/>
+      <c r="DV40"/>
+      <c r="DW40"/>
+      <c r="DX40"/>
+      <c r="DY40"/>
+    </row>
+    <row r="41" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B41" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="E41" s="88"/>
+      <c r="F41" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G41" s="50">
+        <v>45528</v>
+      </c>
+      <c r="H41" s="50">
+        <v>45540</v>
+      </c>
+      <c r="I41" s="17">
+        <v>0</v>
+      </c>
+      <c r="J41" s="18"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="19"/>
+      <c r="O41" s="19"/>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="19"/>
+      <c r="S41" s="19"/>
+      <c r="T41" s="19"/>
+      <c r="U41" s="19"/>
+      <c r="V41" s="19"/>
+      <c r="W41" s="19"/>
+      <c r="X41" s="18"/>
+      <c r="Y41" s="19"/>
+      <c r="Z41" s="19"/>
+      <c r="AA41" s="19"/>
+      <c r="AB41" s="19"/>
+      <c r="AC41" s="19"/>
+      <c r="AD41" s="19"/>
+      <c r="AE41" s="18"/>
+      <c r="AF41" s="19"/>
+      <c r="AG41" s="19"/>
+      <c r="AH41" s="19"/>
+      <c r="AI41" s="19"/>
+      <c r="AJ41" s="19"/>
+      <c r="AK41" s="19"/>
+      <c r="AL41" s="18"/>
+      <c r="AM41" s="19"/>
+      <c r="AN41" s="19"/>
+      <c r="AO41" s="19"/>
+      <c r="AP41" s="19"/>
+      <c r="AQ41" s="19"/>
+      <c r="AR41" s="19"/>
+      <c r="AS41" s="18"/>
+      <c r="AT41" s="19"/>
+      <c r="AU41" s="19"/>
+      <c r="AV41" s="19"/>
+      <c r="AW41" s="19"/>
+      <c r="AX41" s="19"/>
+      <c r="AY41" s="19"/>
+      <c r="AZ41" s="18"/>
+      <c r="BA41" s="19"/>
+      <c r="BB41" s="19"/>
+      <c r="BC41" s="19"/>
+      <c r="BD41" s="19"/>
+      <c r="BE41" s="19"/>
+      <c r="BF41" s="19"/>
+      <c r="BG41" s="18"/>
+      <c r="BH41" s="19"/>
+      <c r="BI41" s="19"/>
+      <c r="BJ41" s="19"/>
+      <c r="BK41" s="63"/>
+    </row>
+    <row r="42" spans="2:129" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B42" s="15"/>
+      <c r="C42" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="107" t="s">
+      <c r="D42" s="111" t="s">
         <v>53</v>
       </c>
-      <c r="E38" s="107"/>
-      <c r="F38" s="37" t="s">
+      <c r="E42" s="111"/>
+      <c r="F42" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="G38" s="68">
+      <c r="G42" s="68">
         <v>45540</v>
       </c>
-      <c r="H38" s="6">
+      <c r="H42" s="6">
         <v>45541</v>
       </c>
-      <c r="I38" s="36">
+      <c r="I42" s="36">
         <v>0</v>
       </c>
-      <c r="J38" s="24"/>
-      <c r="K38" s="25"/>
-      <c r="L38" s="25"/>
-      <c r="M38" s="25"/>
-      <c r="N38" s="25"/>
-      <c r="O38" s="25"/>
-      <c r="P38" s="25"/>
-      <c r="Q38" s="24"/>
-      <c r="R38" s="25"/>
-      <c r="S38" s="25"/>
-      <c r="T38" s="25"/>
-      <c r="U38" s="25"/>
-      <c r="V38" s="25"/>
-      <c r="W38" s="25"/>
-      <c r="X38" s="24"/>
-      <c r="Y38" s="25"/>
-      <c r="Z38" s="25"/>
-      <c r="AA38" s="25"/>
-      <c r="AB38" s="25"/>
-      <c r="AC38" s="25"/>
-      <c r="AD38" s="25"/>
-      <c r="AE38" s="24"/>
-      <c r="AF38" s="25"/>
-      <c r="AG38" s="25"/>
-      <c r="AH38" s="25"/>
-      <c r="AI38" s="25"/>
-      <c r="AJ38" s="25"/>
-      <c r="AK38" s="25"/>
-      <c r="AL38" s="24"/>
-      <c r="AM38" s="25"/>
-      <c r="AN38" s="25"/>
-      <c r="AO38" s="25"/>
-      <c r="AP38" s="25"/>
-      <c r="AQ38" s="25"/>
-      <c r="AR38" s="25"/>
-      <c r="AS38" s="24"/>
-      <c r="AT38" s="25"/>
-      <c r="AU38" s="25"/>
-      <c r="AV38" s="25"/>
-      <c r="AW38" s="25"/>
-      <c r="AX38" s="25"/>
-      <c r="AY38" s="25"/>
-      <c r="AZ38" s="24"/>
-      <c r="BA38" s="25"/>
-      <c r="BB38" s="25"/>
-      <c r="BC38" s="25"/>
-      <c r="BD38" s="25"/>
-      <c r="BE38" s="25"/>
-      <c r="BF38" s="25"/>
-      <c r="BG38" s="24"/>
-      <c r="BH38" s="25"/>
-      <c r="BI38" s="25"/>
-      <c r="BJ38" s="25"/>
-      <c r="BK38" s="69"/>
-      <c r="BL38"/>
-      <c r="BM38"/>
-      <c r="BN38"/>
-      <c r="BO38"/>
-      <c r="BP38"/>
-      <c r="BQ38"/>
-      <c r="BR38"/>
-      <c r="BS38"/>
-      <c r="BT38"/>
-      <c r="BU38"/>
-      <c r="BV38"/>
-      <c r="BW38"/>
-      <c r="BX38"/>
-      <c r="BY38"/>
-      <c r="BZ38"/>
-      <c r="CA38"/>
-      <c r="CB38"/>
-      <c r="CC38"/>
-      <c r="CD38"/>
-      <c r="CE38"/>
-      <c r="CF38"/>
-      <c r="CG38"/>
-      <c r="CH38"/>
-      <c r="CI38"/>
-      <c r="CJ38"/>
-      <c r="CK38"/>
-      <c r="CL38"/>
-      <c r="CM38"/>
-      <c r="CN38"/>
-      <c r="CO38"/>
-      <c r="CP38"/>
-      <c r="CQ38"/>
-      <c r="CR38"/>
-      <c r="CS38"/>
-      <c r="CT38"/>
-      <c r="CU38"/>
-      <c r="CV38"/>
-      <c r="CW38"/>
-      <c r="CX38"/>
-      <c r="CY38"/>
-      <c r="CZ38"/>
-      <c r="DA38"/>
-      <c r="DB38"/>
-      <c r="DC38"/>
-      <c r="DD38"/>
-      <c r="DE38"/>
-      <c r="DF38"/>
-      <c r="DG38"/>
-      <c r="DH38"/>
-      <c r="DI38"/>
-      <c r="DJ38"/>
-      <c r="DK38"/>
-      <c r="DL38"/>
-      <c r="DM38"/>
-      <c r="DN38"/>
-      <c r="DO38"/>
-      <c r="DP38"/>
-      <c r="DQ38"/>
-      <c r="DR38"/>
-      <c r="DS38"/>
-      <c r="DT38"/>
-      <c r="DU38"/>
-      <c r="DV38"/>
-      <c r="DW38"/>
-      <c r="DX38"/>
-      <c r="DY38"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="25"/>
+      <c r="L42" s="25"/>
+      <c r="M42" s="25"/>
+      <c r="N42" s="25"/>
+      <c r="O42" s="25"/>
+      <c r="P42" s="25"/>
+      <c r="Q42" s="24"/>
+      <c r="R42" s="25"/>
+      <c r="S42" s="25"/>
+      <c r="T42" s="25"/>
+      <c r="U42" s="25"/>
+      <c r="V42" s="25"/>
+      <c r="W42" s="25"/>
+      <c r="X42" s="24"/>
+      <c r="Y42" s="25"/>
+      <c r="Z42" s="25"/>
+      <c r="AA42" s="25"/>
+      <c r="AB42" s="25"/>
+      <c r="AC42" s="25"/>
+      <c r="AD42" s="25"/>
+      <c r="AE42" s="24"/>
+      <c r="AF42" s="25"/>
+      <c r="AG42" s="25"/>
+      <c r="AH42" s="25"/>
+      <c r="AI42" s="25"/>
+      <c r="AJ42" s="25"/>
+      <c r="AK42" s="25"/>
+      <c r="AL42" s="24"/>
+      <c r="AM42" s="25"/>
+      <c r="AN42" s="25"/>
+      <c r="AO42" s="25"/>
+      <c r="AP42" s="25"/>
+      <c r="AQ42" s="25"/>
+      <c r="AR42" s="25"/>
+      <c r="AS42" s="24"/>
+      <c r="AT42" s="25"/>
+      <c r="AU42" s="25"/>
+      <c r="AV42" s="25"/>
+      <c r="AW42" s="25"/>
+      <c r="AX42" s="25"/>
+      <c r="AY42" s="25"/>
+      <c r="AZ42" s="24"/>
+      <c r="BA42" s="25"/>
+      <c r="BB42" s="25"/>
+      <c r="BC42" s="25"/>
+      <c r="BD42" s="25"/>
+      <c r="BE42" s="25"/>
+      <c r="BF42" s="25"/>
+      <c r="BG42" s="24"/>
+      <c r="BH42" s="25"/>
+      <c r="BI42" s="25"/>
+      <c r="BJ42" s="25"/>
+      <c r="BK42" s="69"/>
+      <c r="BL42"/>
+      <c r="BM42"/>
+      <c r="BN42"/>
+      <c r="BO42"/>
+      <c r="BP42"/>
+      <c r="BQ42"/>
+      <c r="BR42"/>
+      <c r="BS42"/>
+      <c r="BT42"/>
+      <c r="BU42"/>
+      <c r="BV42"/>
+      <c r="BW42"/>
+      <c r="BX42"/>
+      <c r="BY42"/>
+      <c r="BZ42"/>
+      <c r="CA42"/>
+      <c r="CB42"/>
+      <c r="CC42"/>
+      <c r="CD42"/>
+      <c r="CE42"/>
+      <c r="CF42"/>
+      <c r="CG42"/>
+      <c r="CH42"/>
+      <c r="CI42"/>
+      <c r="CJ42"/>
+      <c r="CK42"/>
+      <c r="CL42"/>
+      <c r="CM42"/>
+      <c r="CN42"/>
+      <c r="CO42"/>
+      <c r="CP42"/>
+      <c r="CQ42"/>
+      <c r="CR42"/>
+      <c r="CS42"/>
+      <c r="CT42"/>
+      <c r="CU42"/>
+      <c r="CV42"/>
+      <c r="CW42"/>
+      <c r="CX42"/>
+      <c r="CY42"/>
+      <c r="CZ42"/>
+      <c r="DA42"/>
+      <c r="DB42"/>
+      <c r="DC42"/>
+      <c r="DD42"/>
+      <c r="DE42"/>
+      <c r="DF42"/>
+      <c r="DG42"/>
+      <c r="DH42"/>
+      <c r="DI42"/>
+      <c r="DJ42"/>
+      <c r="DK42"/>
+      <c r="DL42"/>
+      <c r="DM42"/>
+      <c r="DN42"/>
+      <c r="DO42"/>
+      <c r="DP42"/>
+      <c r="DQ42"/>
+      <c r="DR42"/>
+      <c r="DS42"/>
+      <c r="DT42"/>
+      <c r="DU42"/>
+      <c r="DV42"/>
+      <c r="DW42"/>
+      <c r="DX42"/>
+      <c r="DY42"/>
     </row>
-    <row r="39" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39"/>
-      <c r="F39"/>
-      <c r="G39"/>
-      <c r="H39"/>
-      <c r="I39"/>
-    </row>
-    <row r="40" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40"/>
-      <c r="D40" s="84"/>
-      <c r="E40" s="84"/>
-      <c r="F40"/>
-      <c r="G40"/>
-      <c r="H40"/>
-      <c r="I40"/>
-    </row>
-    <row r="41" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41"/>
-      <c r="D41" s="84"/>
-      <c r="E41" s="84"/>
-      <c r="F41"/>
-      <c r="G41"/>
-      <c r="H41"/>
-      <c r="I41"/>
-    </row>
-    <row r="42" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42"/>
-      <c r="D42" s="84"/>
-      <c r="E42" s="84"/>
-      <c r="F42"/>
-      <c r="G42"/>
-      <c r="H42"/>
-      <c r="I42"/>
-    </row>
-    <row r="43" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B43"/>
-      <c r="D43" s="84"/>
-      <c r="E43" s="84"/>
       <c r="F43"/>
       <c r="G43"/>
       <c r="H43"/>
       <c r="I43"/>
     </row>
-    <row r="44" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B44"/>
-      <c r="D44" s="84"/>
-      <c r="E44" s="84"/>
+      <c r="D44" s="74"/>
+      <c r="E44" s="74"/>
       <c r="F44"/>
       <c r="G44"/>
       <c r="H44"/>
       <c r="I44"/>
     </row>
-    <row r="45" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B45"/>
-      <c r="D45" s="84"/>
-      <c r="E45" s="84"/>
+      <c r="D45" s="74"/>
+      <c r="E45" s="74"/>
       <c r="F45"/>
       <c r="G45"/>
       <c r="H45"/>
       <c r="I45"/>
     </row>
-    <row r="46" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B46"/>
+      <c r="D46" s="74"/>
+      <c r="E46" s="74"/>
       <c r="F46"/>
-      <c r="G46" s="84"/>
-      <c r="H46" s="84"/>
+      <c r="G46"/>
+      <c r="H46"/>
       <c r="I46"/>
     </row>
-    <row r="47" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B47"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="74"/>
       <c r="F47"/>
-      <c r="G47" s="84"/>
-      <c r="H47" s="84"/>
+      <c r="G47"/>
+      <c r="H47"/>
       <c r="I47"/>
     </row>
-    <row r="48" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:129" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B48"/>
-      <c r="D48" s="84"/>
-      <c r="E48" s="84"/>
+      <c r="D48" s="74"/>
+      <c r="E48" s="74"/>
       <c r="F48"/>
       <c r="G48"/>
       <c r="H48"/>
       <c r="I48"/>
     </row>
-    <row r="49" spans="2:48" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:48" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B49"/>
-      <c r="D49" s="84"/>
-      <c r="E49" s="84"/>
+      <c r="D49" s="74"/>
+      <c r="E49" s="74"/>
       <c r="F49"/>
       <c r="G49"/>
       <c r="H49"/>
       <c r="I49"/>
     </row>
-    <row r="50" spans="2:48" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AV50" t="s">
+    <row r="50" spans="2:48" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B50"/>
+      <c r="F50"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="74"/>
+      <c r="I50"/>
+    </row>
+    <row r="51" spans="2:48" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B51"/>
+      <c r="F51"/>
+      <c r="G51" s="74"/>
+      <c r="H51" s="74"/>
+      <c r="I51"/>
+    </row>
+    <row r="52" spans="2:48" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B52"/>
+      <c r="D52" s="74"/>
+      <c r="E52" s="74"/>
+      <c r="F52"/>
+      <c r="G52"/>
+      <c r="H52"/>
+      <c r="I52"/>
+    </row>
+    <row r="53" spans="2:48" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B53"/>
+      <c r="D53" s="74"/>
+      <c r="E53" s="74"/>
+      <c r="F53"/>
+      <c r="G53"/>
+      <c r="H53"/>
+      <c r="I53"/>
+    </row>
+    <row r="54" spans="2:48" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="AV54" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="70">
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:E8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="BN7:BT7"/>
-    <mergeCell ref="BG7:BK7"/>
-    <mergeCell ref="X7:AD7"/>
-    <mergeCell ref="AE7:AK7"/>
-    <mergeCell ref="AL7:AR7"/>
+  <mergeCells count="74">
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="C13:C19"/>
+    <mergeCell ref="G29:G34"/>
+    <mergeCell ref="H29:H34"/>
+    <mergeCell ref="G35:G40"/>
+    <mergeCell ref="H35:H40"/>
+    <mergeCell ref="H20:H26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="C35:C40"/>
+    <mergeCell ref="C29:C34"/>
+    <mergeCell ref="C20:C26"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
     <mergeCell ref="D49:E49"/>
-    <mergeCell ref="J7:P7"/>
-    <mergeCell ref="Q7:W7"/>
-    <mergeCell ref="D9:E11"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="H46:H47"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="G13:G19"/>
+    <mergeCell ref="G20:G26"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
     <mergeCell ref="AA5:BE5"/>
     <mergeCell ref="BF5:BK5"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="F9:F11"/>
     <mergeCell ref="D14:E14"/>
-    <mergeCell ref="H13:H18"/>
-    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="H13:H19"/>
+    <mergeCell ref="D19:E19"/>
     <mergeCell ref="AS7:AY7"/>
     <mergeCell ref="AZ7:BF7"/>
     <mergeCell ref="I7:I8"/>
@@ -5493,35 +5994,32 @@
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="G13:G18"/>
-    <mergeCell ref="G19:G24"/>
-    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="J7:P7"/>
+    <mergeCell ref="Q7:W7"/>
+    <mergeCell ref="D9:E11"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="H50:H51"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="C13:C18"/>
-    <mergeCell ref="G27:G31"/>
-    <mergeCell ref="H27:H31"/>
-    <mergeCell ref="G32:G36"/>
-    <mergeCell ref="H32:H36"/>
-    <mergeCell ref="H19:H24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="C19:C24"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="BN7:BT7"/>
+    <mergeCell ref="BG7:BK7"/>
+    <mergeCell ref="X7:AD7"/>
+    <mergeCell ref="AE7:AK7"/>
+    <mergeCell ref="AL7:AR7"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:E8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>